<commit_message>
root words dataset reformed
</commit_message>
<xml_diff>
--- a/root_words.xlsx
+++ b/root_words.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="10835" windowHeight="9072"/>
+    <workbookView windowWidth="10908" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="800">
   <si>
     <t>word</t>
   </si>
@@ -1933,364 +1933,487 @@
     <t>বিশাল</t>
   </si>
   <si>
+    <t>সমাধি</t>
+  </si>
+  <si>
+    <t>কোটি</t>
+  </si>
+  <si>
+    <t>জন</t>
+  </si>
+  <si>
+    <t>অধ্যুষিত</t>
+  </si>
+  <si>
+    <t>নিদারুণ</t>
+  </si>
+  <si>
+    <t>অভাব</t>
+  </si>
+  <si>
+    <t>অনটন</t>
+  </si>
+  <si>
+    <t>নিপীড়ন</t>
+  </si>
+  <si>
+    <t>অনেক</t>
+  </si>
+  <si>
+    <t>নিরক্ষর</t>
+  </si>
+  <si>
+    <t>নিবিড়</t>
+  </si>
+  <si>
+    <t>অন্ধকার</t>
+  </si>
+  <si>
+    <t>নিমজ্জিত</t>
+  </si>
+  <si>
+    <t>এর</t>
+  </si>
+  <si>
+    <t>আছে</t>
+  </si>
+  <si>
+    <t>বিপর্যয়</t>
+  </si>
+  <si>
+    <t>ঝঞ্ঝা</t>
+  </si>
+  <si>
+    <t>ঝড়ঝঞ্ঝা</t>
+  </si>
+  <si>
+    <t>খরা</t>
+  </si>
+  <si>
+    <t>ভূমিকম্প</t>
+  </si>
+  <si>
+    <t>দুর্ভিক্ষ</t>
+  </si>
+  <si>
+    <t>মহামারী</t>
+  </si>
+  <si>
+    <t>তান্ডব</t>
+  </si>
+  <si>
+    <t>লীলা</t>
+  </si>
+  <si>
+    <t>বাহুল্য</t>
+  </si>
+  <si>
+    <t>এদেশ</t>
+  </si>
+  <si>
+    <t>বিদেশ</t>
+  </si>
+  <si>
+    <t>এসব</t>
+  </si>
+  <si>
+    <t>দুর্যোগ</t>
+  </si>
+  <si>
+    <t>মোকাবিলা</t>
+  </si>
+  <si>
+    <t>প্রাথমিক</t>
+  </si>
+  <si>
+    <t>দায়িত্ব</t>
+  </si>
+  <si>
+    <t>সরকার</t>
+  </si>
+  <si>
+    <t>জনকল্যাণমুখী</t>
+  </si>
+  <si>
+    <t>জনকল্যাণ</t>
+  </si>
+  <si>
+    <t>গণতন্ত্র</t>
+  </si>
+  <si>
+    <t>কিন্তু</t>
+  </si>
+  <si>
+    <t>কী</t>
+  </si>
+  <si>
+    <t>অর্থ</t>
+  </si>
+  <si>
+    <t>কি</t>
+  </si>
+  <si>
+    <t>সামর্থ্য</t>
+  </si>
+  <si>
+    <t>বিরাট</t>
+  </si>
+  <si>
+    <t>সমাধান</t>
+  </si>
+  <si>
+    <t>রাষ্ট্রশক্তি</t>
+  </si>
+  <si>
+    <t>কখন</t>
+  </si>
+  <si>
+    <t>নয়</t>
+  </si>
+  <si>
+    <t>সেই</t>
+  </si>
+  <si>
+    <t>সে</t>
+  </si>
+  <si>
+    <t>দিক</t>
+  </si>
+  <si>
+    <t>অপরিসীম</t>
+  </si>
+  <si>
+    <t>আমরা</t>
+  </si>
+  <si>
+    <t>একা</t>
+  </si>
+  <si>
+    <t>সভ্য</t>
+  </si>
+  <si>
+    <t>পর</t>
+  </si>
+  <si>
+    <t>ভারত</t>
+  </si>
+  <si>
+    <t>সুপ্রাচীন</t>
+  </si>
+  <si>
+    <t>উপমহাদেশ</t>
+  </si>
+  <si>
+    <t>অর্থনীতি</t>
+  </si>
+  <si>
+    <t>ঐতিহ্য</t>
+  </si>
+  <si>
+    <t>জন্য</t>
+  </si>
+  <si>
+    <t>সুপরিচিত</t>
+  </si>
+  <si>
+    <t>সিন্ধু</t>
+  </si>
+  <si>
+    <t>বিভিন্ন</t>
+  </si>
+  <si>
+    <t>পর্ব</t>
+  </si>
+  <si>
+    <t>স্থাপিত</t>
+  </si>
+  <si>
+    <t>বিশালাকার</t>
+  </si>
+  <si>
+    <t>একাধিক</t>
+  </si>
+  <si>
+    <t>সাম্রাজ্য</t>
+  </si>
+  <si>
+    <t>নানা</t>
+  </si>
+  <si>
+    <t>সভা</t>
+  </si>
+  <si>
+    <t>প্রসিদ্ধ</t>
+  </si>
+  <si>
+    <t>বাণিজ্যপথ</t>
+  </si>
+  <si>
+    <t>অন্যান্য</t>
+  </si>
+  <si>
+    <t>বাণিজ্য</t>
+  </si>
+  <si>
+    <t>সম্পর্ক</t>
+  </si>
+  <si>
+    <t>রক্ষা</t>
+  </si>
+  <si>
+    <t>হিন্দু</t>
+  </si>
+  <si>
+    <t>বৌদ্ধ</t>
+  </si>
+  <si>
+    <t>জৈন</t>
+  </si>
+  <si>
+    <t>শিখ</t>
+  </si>
+  <si>
+    <t>উৎসভূমি</t>
+  </si>
+  <si>
+    <t>খ্রিস্ট</t>
+  </si>
+  <si>
+    <t>সহস্রাব্দ</t>
+  </si>
+  <si>
+    <t>পারসি</t>
+  </si>
+  <si>
+    <t>ইহুদি</t>
+  </si>
+  <si>
+    <t>প্রবেশ</t>
+  </si>
+  <si>
+    <t>প্রভাব</t>
+  </si>
+  <si>
+    <t>অষ্টাদশ</t>
+  </si>
+  <si>
+    <t>শতাব্দী</t>
+  </si>
+  <si>
+    <t>প্রথমার্ধ</t>
+  </si>
+  <si>
+    <t>ব্রিটিশ</t>
+  </si>
+  <si>
+    <t>ইস্ট</t>
+  </si>
+  <si>
+    <t>ইন্ডিয়া</t>
+  </si>
+  <si>
+    <t>কোম্পানি</t>
+  </si>
+  <si>
+    <t>ভূখণ্ড</t>
+  </si>
+  <si>
+    <t>অধিকাংশ</t>
+  </si>
+  <si>
+    <t>শাসনাধীন</t>
+  </si>
+  <si>
+    <t>আনা</t>
+  </si>
+  <si>
+    <t>সক্ষম</t>
+  </si>
+  <si>
+    <t>উনবিংশ</t>
+  </si>
+  <si>
+    <t>ইসলাম</t>
+  </si>
+  <si>
+    <t>খ্রিস্টধর্ম</t>
+  </si>
+  <si>
+    <t>মধ্যভাগ</t>
+  </si>
+  <si>
+    <t>পুরোদস্তুর</t>
+  </si>
+  <si>
+    <t>উপনিবেশ</t>
+  </si>
+  <si>
+    <t>পরিণত</t>
+  </si>
+  <si>
+    <t>অতঃপর</t>
+  </si>
+  <si>
+    <t>সংগ্রাম</t>
+  </si>
+  <si>
+    <t>সাল</t>
+  </si>
+  <si>
+    <t>স্বতন্ত্র</t>
+  </si>
+  <si>
+    <t>রাষ্ট্ররূপ</t>
+  </si>
+  <si>
+    <t>আত্মপ্রকাশ</t>
+  </si>
+  <si>
+    <t>সংবিধান</t>
+  </si>
+  <si>
+    <t>প্রণয়ন</t>
+  </si>
+  <si>
+    <t>মাধ্যম</t>
+  </si>
+  <si>
+    <t>সার্বভৌম</t>
+  </si>
+  <si>
+    <t>গণতান্ত্রিক</t>
+  </si>
+  <si>
+    <t>প্রজাতন্ত্র</t>
+  </si>
+  <si>
+    <t>সুদীর্ঘ</t>
+  </si>
+  <si>
+    <t>গরিষ্ঠ</t>
+  </si>
+  <si>
+    <t>ক্ষেত্র</t>
+  </si>
+  <si>
+    <t>বহুদূর</t>
+  </si>
+  <si>
+    <t>বিস্তৃত</t>
+  </si>
+  <si>
+    <t>অংশগ্রহণ</t>
+  </si>
+  <si>
+    <t>কে</t>
+  </si>
+  <si>
+    <t>কারা</t>
+  </si>
+  <si>
+    <t>অবশ্য</t>
+  </si>
+  <si>
+    <t>ভূমিকা</t>
+  </si>
+  <si>
+    <t>অগ্রগণ্য</t>
+  </si>
+  <si>
+    <t>অসংখ্য</t>
+  </si>
+  <si>
+    <t>জনহিতকর</t>
+  </si>
+  <si>
+    <t>গুলি</t>
+  </si>
+  <si>
+    <t>নগণ্য</t>
+  </si>
+  <si>
+    <t>সমাজসেবামূলক</t>
+  </si>
+  <si>
+    <t>রামকৃষ্ণ</t>
+  </si>
+  <si>
+    <t>মিশন</t>
+  </si>
+  <si>
+    <t>সেবাশ্রম</t>
+  </si>
+  <si>
+    <t>মাড়োয়ারি</t>
+  </si>
+  <si>
+    <t>রিলিফ</t>
+  </si>
+  <si>
+    <t>সোসাইটি</t>
+  </si>
+  <si>
+    <t>রেড</t>
+  </si>
+  <si>
+    <t>ক্রস</t>
+  </si>
+  <si>
+    <t>সেন্ট</t>
+  </si>
+  <si>
+    <t>জনস্</t>
+  </si>
+  <si>
+    <t>অ্যাম্বুলেন্স</t>
+  </si>
+  <si>
+    <t>প্রভৃতি</t>
+  </si>
+  <si>
+    <t>উল্লেখযোগ্য</t>
+  </si>
+  <si>
+    <t>অকুণ্ঠ</t>
+  </si>
+  <si>
+    <t>নিরলস</t>
+  </si>
+  <si>
+    <t>জনসেবা</t>
+  </si>
+  <si>
+    <t>বিপুল</t>
+  </si>
+  <si>
+    <t>তুলনা</t>
+  </si>
+  <si>
+    <t>বৃহত্তর</t>
+  </si>
+  <si>
+    <t>বহন</t>
+  </si>
+  <si>
+    <t>পালন</t>
+  </si>
+  <si>
+    <t>গুরু</t>
+  </si>
+  <si>
     <t>গুরুত্ব</t>
   </si>
   <si>
-    <t>সমাধি</t>
-  </si>
-  <si>
-    <t>কোটি</t>
-  </si>
-  <si>
-    <t>জন</t>
-  </si>
-  <si>
-    <t>অধ্যুষিত</t>
-  </si>
-  <si>
-    <t>নিদারুণ</t>
-  </si>
-  <si>
-    <t>অভাব</t>
-  </si>
-  <si>
-    <t>অনটন</t>
-  </si>
-  <si>
-    <t>নিপীড়ন</t>
-  </si>
-  <si>
-    <t>অনেক</t>
-  </si>
-  <si>
-    <t>নিরক্ষর</t>
-  </si>
-  <si>
-    <t>নিবিড়</t>
-  </si>
-  <si>
-    <t>অন্ধকার</t>
-  </si>
-  <si>
-    <t>নিমজ্জিত</t>
-  </si>
-  <si>
-    <t>এর</t>
-  </si>
-  <si>
-    <t>আছে</t>
-  </si>
-  <si>
-    <t>বিপর্যয়</t>
-  </si>
-  <si>
-    <t>ঝঞ্ঝা</t>
-  </si>
-  <si>
-    <t>ঝড়ঝঞ্ঝা</t>
-  </si>
-  <si>
-    <t>খরা</t>
-  </si>
-  <si>
-    <t>ভূমিকম্প</t>
-  </si>
-  <si>
-    <t>দুর্ভিক্ষ</t>
-  </si>
-  <si>
-    <t>মহামারী</t>
-  </si>
-  <si>
-    <t>তান্ডব</t>
-  </si>
-  <si>
-    <t>লীলা</t>
-  </si>
-  <si>
-    <t>বাহুল্য</t>
-  </si>
-  <si>
-    <t>এদেশ</t>
-  </si>
-  <si>
-    <t>বিদেশ</t>
-  </si>
-  <si>
-    <t>এসব</t>
-  </si>
-  <si>
-    <t>দুর্যোগ</t>
-  </si>
-  <si>
-    <t>মোকাবিলা</t>
-  </si>
-  <si>
-    <t>প্রাথমিক</t>
-  </si>
-  <si>
-    <t>দায়িত্ব</t>
-  </si>
-  <si>
-    <t>সরকার</t>
-  </si>
-  <si>
-    <t>জনকল্যাণমুখী</t>
-  </si>
-  <si>
-    <t>জনকল্যাণ</t>
-  </si>
-  <si>
-    <t>গণতন্ত্র</t>
-  </si>
-  <si>
-    <t>কিন্তু</t>
-  </si>
-  <si>
-    <t>কী</t>
-  </si>
-  <si>
-    <t>অর্থ</t>
-  </si>
-  <si>
-    <t>কি</t>
-  </si>
-  <si>
-    <t>সামর্থ্য</t>
-  </si>
-  <si>
-    <t>বিরাট</t>
-  </si>
-  <si>
-    <t>সমাধান</t>
-  </si>
-  <si>
-    <t>রাষ্ট্রশক্তি</t>
-  </si>
-  <si>
-    <t>কখন</t>
-  </si>
-  <si>
-    <t>নয়</t>
-  </si>
-  <si>
-    <t>সেই</t>
-  </si>
-  <si>
-    <t>সে</t>
-  </si>
-  <si>
-    <t>দিক</t>
-  </si>
-  <si>
-    <t>অপরিসীম</t>
-  </si>
-  <si>
-    <t>আমরা</t>
-  </si>
-  <si>
-    <t>একা</t>
-  </si>
-  <si>
-    <t>সভ্য</t>
-  </si>
-  <si>
-    <t>পর</t>
-  </si>
-  <si>
-    <t>ভারত</t>
-  </si>
-  <si>
-    <t>সুপ্রাচীন</t>
-  </si>
-  <si>
-    <t>উপমহাদেশ</t>
-  </si>
-  <si>
-    <t>অর্থনীতি</t>
-  </si>
-  <si>
-    <t>ঐতিহ্য</t>
-  </si>
-  <si>
-    <t>জন্য</t>
-  </si>
-  <si>
-    <t>সুপরিচিত</t>
-  </si>
-  <si>
-    <t>সিন্ধু</t>
-  </si>
-  <si>
-    <t>বিভিন্ন</t>
-  </si>
-  <si>
-    <t>পর্ব</t>
-  </si>
-  <si>
-    <t>স্থাপিত</t>
-  </si>
-  <si>
-    <t>বিশালাকার</t>
-  </si>
-  <si>
-    <t>একাধিক</t>
-  </si>
-  <si>
-    <t>সাম্রাজ্য</t>
-  </si>
-  <si>
-    <t>নানা</t>
-  </si>
-  <si>
-    <t>সভা</t>
-  </si>
-  <si>
-    <t>প্রসিদ্ধ</t>
-  </si>
-  <si>
-    <t>বাণিজ্যপথ</t>
-  </si>
-  <si>
-    <t>অন্যান্য</t>
-  </si>
-  <si>
-    <t>বাণিজ্য</t>
-  </si>
-  <si>
-    <t>সম্পর্ক</t>
-  </si>
-  <si>
-    <t>রক্ষা</t>
-  </si>
-  <si>
-    <t>হিন্দু</t>
-  </si>
-  <si>
-    <t>বৌদ্ধ</t>
-  </si>
-  <si>
-    <t>জৈন</t>
-  </si>
-  <si>
-    <t>শিখ</t>
-  </si>
-  <si>
-    <t>উৎসভূমি</t>
-  </si>
-  <si>
-    <t>খ্রিস্ট</t>
-  </si>
-  <si>
-    <t>সহস্রাব্দ</t>
-  </si>
-  <si>
-    <t>পারসি</t>
-  </si>
-  <si>
-    <t>ইহুদি</t>
-  </si>
-  <si>
-    <t>প্রবেশ</t>
-  </si>
-  <si>
-    <t>প্রভাব</t>
-  </si>
-  <si>
-    <t>অষ্টাদশ</t>
-  </si>
-  <si>
-    <t>শতাব্দী</t>
-  </si>
-  <si>
-    <t>প্রথমার্ধ</t>
-  </si>
-  <si>
-    <t>ব্রিটিশ</t>
-  </si>
-  <si>
-    <t>ইস্ট</t>
-  </si>
-  <si>
-    <t>ইন্ডিয়া</t>
-  </si>
-  <si>
-    <t>কোম্পানি</t>
-  </si>
-  <si>
-    <t>ভূখণ্ড</t>
-  </si>
-  <si>
-    <t>অধিকাংশ</t>
-  </si>
-  <si>
-    <t>শাসনাধীন</t>
-  </si>
-  <si>
-    <t>আনা</t>
-  </si>
-  <si>
-    <t>সক্ষম</t>
-  </si>
-  <si>
-    <t>উনবিংশ</t>
-  </si>
-  <si>
-    <t>ইসলাম</t>
-  </si>
-  <si>
-    <t>খ্রিস্টধর্ম</t>
-  </si>
-  <si>
-    <t>মধ্যভাগ</t>
-  </si>
-  <si>
-    <t>পুরোদস্তুর</t>
-  </si>
-  <si>
-    <t>উপনিবেশ</t>
-  </si>
-  <si>
-    <t>পরিণত</t>
-  </si>
-  <si>
-    <t>অতঃপর</t>
-  </si>
-  <si>
-    <t>সংগ্রাম</t>
-  </si>
-  <si>
-    <t>সাল</t>
-  </si>
-  <si>
-    <t>স্বতন্ত্র</t>
-  </si>
-  <si>
-    <t>রাষ্ট্ররূপ</t>
-  </si>
-  <si>
-    <t>আত্মপ্রকাশ</t>
-  </si>
-  <si>
-    <t>সংবিধান</t>
-  </si>
-  <si>
-    <t>প্রণয়ন</t>
-  </si>
-  <si>
-    <t>মাধ্যম</t>
-  </si>
-  <si>
-    <t>সার্বভৌম</t>
-  </si>
-  <si>
-    <t>গণতান্ত্রিক</t>
-  </si>
-  <si>
-    <t>প্রজাতন্ত্র</t>
-  </si>
-  <si>
-    <t>সুদীর্ঘ</t>
+    <t>ভার</t>
+  </si>
+  <si>
+    <t>তবে</t>
+  </si>
+  <si>
+    <t>পর্যাপ্ত</t>
+  </si>
+  <si>
+    <t>বা</t>
   </si>
 </sst>
 </file>
@@ -2298,10 +2421,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -2342,16 +2465,22 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2359,6 +2488,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2372,40 +2516,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2425,9 +2540,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2441,6 +2587,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
@@ -2449,38 +2603,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2495,7 +2618,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2507,7 +2654,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2519,31 +2696,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2561,25 +2738,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2591,31 +2756,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2627,55 +2798,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2704,6 +2827,54 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2721,33 +2892,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2775,177 +2924,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3321,10 +3444,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:X999"/>
+  <dimension ref="A1:X997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A468" workbookViewId="0">
-      <selection activeCell="A470" sqref="$A470:$XFD470"/>
+    <sheetView tabSelected="1" topLeftCell="A799" workbookViewId="0">
+      <selection activeCell="A812" sqref="A812"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -21339,7 +21462,7 @@
       <c r="X643" s="3"/>
     </row>
     <row r="644" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A644" s="5" t="s">
+      <c r="A644" s="7" t="s">
         <v>639</v>
       </c>
       <c r="B644" s="3"/>
@@ -21367,7 +21490,7 @@
       <c r="X644" s="3"/>
     </row>
     <row r="645" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A645" s="7" t="s">
+      <c r="A645" s="4" t="s">
         <v>640</v>
       </c>
       <c r="B645" s="3"/>
@@ -21395,7 +21518,7 @@
       <c r="X645" s="3"/>
     </row>
     <row r="646" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A646" s="4" t="s">
+      <c r="A646" s="7" t="s">
         <v>641</v>
       </c>
       <c r="B646" s="3"/>
@@ -21423,7 +21546,7 @@
       <c r="X646" s="3"/>
     </row>
     <row r="647" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A647" s="7" t="s">
+      <c r="A647" s="4" t="s">
         <v>642</v>
       </c>
       <c r="B647" s="3"/>
@@ -21480,7 +21603,7 @@
     </row>
     <row r="649" ht="18.75" customHeight="1" spans="1:24">
       <c r="A649" s="4" t="s">
-        <v>644</v>
+        <v>233</v>
       </c>
       <c r="B649" s="3"/>
       <c r="C649" s="3"/>
@@ -21507,8 +21630,8 @@
       <c r="X649" s="3"/>
     </row>
     <row r="650" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A650" s="4" t="s">
-        <v>233</v>
+      <c r="A650" s="7" t="s">
+        <v>644</v>
       </c>
       <c r="B650" s="3"/>
       <c r="C650" s="3"/>
@@ -21535,7 +21658,7 @@
       <c r="X650" s="3"/>
     </row>
     <row r="651" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A651" s="7" t="s">
+      <c r="A651" s="4" t="s">
         <v>645</v>
       </c>
       <c r="B651" s="3"/>
@@ -21647,7 +21770,7 @@
       <c r="X654" s="3"/>
     </row>
     <row r="655" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A655" s="4" t="s">
+      <c r="A655" s="5" t="s">
         <v>649</v>
       </c>
       <c r="B655" s="3"/>
@@ -21703,7 +21826,7 @@
       <c r="X656" s="3"/>
     </row>
     <row r="657" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A657" s="5" t="s">
+      <c r="A657" s="4" t="s">
         <v>651</v>
       </c>
       <c r="B657" s="3"/>
@@ -21731,7 +21854,7 @@
       <c r="X657" s="3"/>
     </row>
     <row r="658" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A658" s="4" t="s">
+      <c r="A658" s="7" t="s">
         <v>652</v>
       </c>
       <c r="B658" s="3"/>
@@ -21759,7 +21882,7 @@
       <c r="X658" s="3"/>
     </row>
     <row r="659" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A659" s="7" t="s">
+      <c r="A659" s="4" t="s">
         <v>653</v>
       </c>
       <c r="B659" s="3"/>
@@ -21871,7 +21994,7 @@
       <c r="X662" s="3"/>
     </row>
     <row r="663" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A663" s="4" t="s">
+      <c r="A663" s="5" t="s">
         <v>657</v>
       </c>
       <c r="B663" s="3"/>
@@ -21899,7 +22022,7 @@
       <c r="X663" s="3"/>
     </row>
     <row r="664" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A664" s="5" t="s">
+      <c r="A664" s="4" t="s">
         <v>658</v>
       </c>
       <c r="B664" s="3"/>
@@ -22039,7 +22162,7 @@
       <c r="X668" s="3"/>
     </row>
     <row r="669" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A669" s="4" t="s">
+      <c r="A669" s="5" t="s">
         <v>663</v>
       </c>
       <c r="B669" s="3"/>
@@ -22067,7 +22190,7 @@
       <c r="X669" s="3"/>
     </row>
     <row r="670" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A670" s="5" t="s">
+      <c r="A670" s="4" t="s">
         <v>664</v>
       </c>
       <c r="B670" s="3"/>
@@ -22152,7 +22275,7 @@
     </row>
     <row r="673" ht="18.75" customHeight="1" spans="1:24">
       <c r="A673" s="4" t="s">
-        <v>667</v>
+        <v>478</v>
       </c>
       <c r="B673" s="3"/>
       <c r="C673" s="3"/>
@@ -22180,7 +22303,7 @@
     </row>
     <row r="674" ht="18.75" customHeight="1" spans="1:24">
       <c r="A674" s="4" t="s">
-        <v>478</v>
+        <v>667</v>
       </c>
       <c r="B674" s="3"/>
       <c r="C674" s="3"/>
@@ -22208,7 +22331,7 @@
     </row>
     <row r="675" ht="18.75" customHeight="1" spans="1:24">
       <c r="A675" s="4" t="s">
-        <v>668</v>
+        <v>652</v>
       </c>
       <c r="B675" s="3"/>
       <c r="C675" s="3"/>
@@ -22236,7 +22359,7 @@
     </row>
     <row r="676" ht="18.75" customHeight="1" spans="1:24">
       <c r="A676" s="4" t="s">
-        <v>653</v>
+        <v>668</v>
       </c>
       <c r="B676" s="3"/>
       <c r="C676" s="3"/>
@@ -22515,7 +22638,7 @@
       <c r="X685" s="3"/>
     </row>
     <row r="686" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A686" s="4" t="s">
+      <c r="A686" s="7" t="s">
         <v>678</v>
       </c>
       <c r="B686" s="3"/>
@@ -22571,7 +22694,7 @@
       <c r="X687" s="3"/>
     </row>
     <row r="688" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A688" s="7" t="s">
+      <c r="A688" s="4" t="s">
         <v>680</v>
       </c>
       <c r="B688" s="3"/>
@@ -22656,7 +22779,7 @@
     </row>
     <row r="691" ht="18.75" customHeight="1" spans="1:24">
       <c r="A691" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B691" s="3"/>
       <c r="C691" s="3"/>
@@ -22739,7 +22862,7 @@
       <c r="X693" s="3"/>
     </row>
     <row r="694" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A694" s="4" t="s">
+      <c r="A694" s="5" t="s">
         <v>685</v>
       </c>
       <c r="B694" s="3"/>
@@ -22767,7 +22890,7 @@
       <c r="X694" s="3"/>
     </row>
     <row r="695" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A695" s="5" t="s">
+      <c r="A695" s="4" t="s">
         <v>686</v>
       </c>
       <c r="B695" s="3"/>
@@ -22851,8 +22974,8 @@
       <c r="X697" s="3"/>
     </row>
     <row r="698" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A698" s="4" t="s">
-        <v>639</v>
+      <c r="A698" s="7" t="s">
+        <v>689</v>
       </c>
       <c r="B698" s="3"/>
       <c r="C698" s="3"/>
@@ -22880,7 +23003,7 @@
     </row>
     <row r="699" ht="18.75" customHeight="1" spans="1:24">
       <c r="A699" s="4" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="B699" s="3"/>
       <c r="C699" s="3"/>
@@ -22907,8 +23030,8 @@
       <c r="X699" s="3"/>
     </row>
     <row r="700" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A700" s="7" t="s">
-        <v>690</v>
+      <c r="A700" s="4" t="s">
+        <v>99</v>
       </c>
       <c r="B700" s="3"/>
       <c r="C700" s="3"/>
@@ -22935,7 +23058,7 @@
       <c r="X700" s="3"/>
     </row>
     <row r="701" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A701" s="4" t="s">
+      <c r="A701" s="8" t="s">
         <v>691</v>
       </c>
       <c r="B701" s="3"/>
@@ -22964,7 +23087,7 @@
     </row>
     <row r="702" ht="18.75" customHeight="1" spans="1:24">
       <c r="A702" s="4" t="s">
-        <v>99</v>
+        <v>692</v>
       </c>
       <c r="B702" s="3"/>
       <c r="C702" s="3"/>
@@ -22991,8 +23114,8 @@
       <c r="X702" s="3"/>
     </row>
     <row r="703" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A703" s="8" t="s">
-        <v>692</v>
+      <c r="A703" s="4" t="s">
+        <v>693</v>
       </c>
       <c r="B703" s="3"/>
       <c r="C703" s="3"/>
@@ -23020,7 +23143,7 @@
     </row>
     <row r="704" ht="18.75" customHeight="1" spans="1:24">
       <c r="A704" s="4" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="B704" s="3"/>
       <c r="C704" s="3"/>
@@ -23048,7 +23171,7 @@
     </row>
     <row r="705" ht="18.75" customHeight="1" spans="1:24">
       <c r="A705" s="4" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="B705" s="3"/>
       <c r="C705" s="3"/>
@@ -23076,7 +23199,7 @@
     </row>
     <row r="706" ht="18.75" customHeight="1" spans="1:24">
       <c r="A706" s="4" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="B706" s="3"/>
       <c r="C706" s="3"/>
@@ -23104,7 +23227,7 @@
     </row>
     <row r="707" ht="18.75" customHeight="1" spans="1:24">
       <c r="A707" s="4" t="s">
-        <v>696</v>
+        <v>493</v>
       </c>
       <c r="B707" s="3"/>
       <c r="C707" s="3"/>
@@ -23160,7 +23283,7 @@
     </row>
     <row r="709" ht="18.75" customHeight="1" spans="1:24">
       <c r="A709" s="4" t="s">
-        <v>493</v>
+        <v>698</v>
       </c>
       <c r="B709" s="3"/>
       <c r="C709" s="3"/>
@@ -23188,7 +23311,7 @@
     </row>
     <row r="710" ht="18.75" customHeight="1" spans="1:24">
       <c r="A710" s="4" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="B710" s="3"/>
       <c r="C710" s="3"/>
@@ -23216,7 +23339,7 @@
     </row>
     <row r="711" ht="18.75" customHeight="1" spans="1:24">
       <c r="A711" s="4" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="B711" s="3"/>
       <c r="C711" s="3"/>
@@ -23244,7 +23367,7 @@
     </row>
     <row r="712" ht="18.75" customHeight="1" spans="1:24">
       <c r="A712" s="4" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="B712" s="3"/>
       <c r="C712" s="3"/>
@@ -23272,7 +23395,7 @@
     </row>
     <row r="713" ht="18.75" customHeight="1" spans="1:24">
       <c r="A713" s="4" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="B713" s="3"/>
       <c r="C713" s="3"/>
@@ -23300,7 +23423,7 @@
     </row>
     <row r="714" ht="18.75" customHeight="1" spans="1:24">
       <c r="A714" s="4" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="B714" s="3"/>
       <c r="C714" s="3"/>
@@ -23328,7 +23451,7 @@
     </row>
     <row r="715" ht="18.75" customHeight="1" spans="1:24">
       <c r="A715" s="4" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="B715" s="3"/>
       <c r="C715" s="3"/>
@@ -23356,7 +23479,7 @@
     </row>
     <row r="716" ht="18.75" customHeight="1" spans="1:24">
       <c r="A716" s="4" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B716" s="3"/>
       <c r="C716" s="3"/>
@@ -23384,7 +23507,7 @@
     </row>
     <row r="717" ht="18.75" customHeight="1" spans="1:24">
       <c r="A717" s="4" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="B717" s="3"/>
       <c r="C717" s="3"/>
@@ -23412,7 +23535,7 @@
     </row>
     <row r="718" ht="18.75" customHeight="1" spans="1:24">
       <c r="A718" s="4" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="B718" s="3"/>
       <c r="C718" s="3"/>
@@ -23440,7 +23563,7 @@
     </row>
     <row r="719" ht="18.75" customHeight="1" spans="1:24">
       <c r="A719" s="4" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="B719" s="3"/>
       <c r="C719" s="3"/>
@@ -23468,7 +23591,7 @@
     </row>
     <row r="720" ht="18.75" customHeight="1" spans="1:24">
       <c r="A720" s="4" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="B720" s="3"/>
       <c r="C720" s="3"/>
@@ -23496,7 +23619,7 @@
     </row>
     <row r="721" ht="18.75" customHeight="1" spans="1:24">
       <c r="A721" s="4" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="B721" s="3"/>
       <c r="C721" s="3"/>
@@ -23524,7 +23647,7 @@
     </row>
     <row r="722" ht="18.75" customHeight="1" spans="1:24">
       <c r="A722" s="4" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B722" s="3"/>
       <c r="C722" s="3"/>
@@ -23552,7 +23675,7 @@
     </row>
     <row r="723" ht="18.75" customHeight="1" spans="1:24">
       <c r="A723" s="4" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="B723" s="3"/>
       <c r="C723" s="3"/>
@@ -23580,7 +23703,7 @@
     </row>
     <row r="724" ht="18.75" customHeight="1" spans="1:24">
       <c r="A724" s="4" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="B724" s="3"/>
       <c r="C724" s="3"/>
@@ -23608,7 +23731,7 @@
     </row>
     <row r="725" ht="18.75" customHeight="1" spans="1:24">
       <c r="A725" s="4" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="B725" s="3"/>
       <c r="C725" s="3"/>
@@ -23636,7 +23759,7 @@
     </row>
     <row r="726" ht="18.75" customHeight="1" spans="1:24">
       <c r="A726" s="4" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="B726" s="3"/>
       <c r="C726" s="3"/>
@@ -23664,7 +23787,7 @@
     </row>
     <row r="727" ht="18.75" customHeight="1" spans="1:24">
       <c r="A727" s="4" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="B727" s="3"/>
       <c r="C727" s="3"/>
@@ -23692,7 +23815,7 @@
     </row>
     <row r="728" ht="18.75" customHeight="1" spans="1:24">
       <c r="A728" s="4" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="B728" s="3"/>
       <c r="C728" s="3"/>
@@ -23720,7 +23843,7 @@
     </row>
     <row r="729" ht="18.75" customHeight="1" spans="1:24">
       <c r="A729" s="4" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="B729" s="3"/>
       <c r="C729" s="3"/>
@@ -23748,7 +23871,7 @@
     </row>
     <row r="730" ht="18.75" customHeight="1" spans="1:24">
       <c r="A730" s="4" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="B730" s="3"/>
       <c r="C730" s="3"/>
@@ -23776,7 +23899,7 @@
     </row>
     <row r="731" ht="18.75" customHeight="1" spans="1:24">
       <c r="A731" s="4" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="B731" s="3"/>
       <c r="C731" s="3"/>
@@ -23804,7 +23927,7 @@
     </row>
     <row r="732" ht="18.75" customHeight="1" spans="1:24">
       <c r="A732" s="4" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="B732" s="3"/>
       <c r="C732" s="3"/>
@@ -23832,7 +23955,7 @@
     </row>
     <row r="733" ht="18.75" customHeight="1" spans="1:24">
       <c r="A733" s="4" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B733" s="3"/>
       <c r="C733" s="3"/>
@@ -23860,7 +23983,7 @@
     </row>
     <row r="734" ht="18.75" customHeight="1" spans="1:24">
       <c r="A734" s="4" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="B734" s="3"/>
       <c r="C734" s="3"/>
@@ -23888,7 +24011,7 @@
     </row>
     <row r="735" ht="18.75" customHeight="1" spans="1:24">
       <c r="A735" s="4" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="B735" s="3"/>
       <c r="C735" s="3"/>
@@ -23916,7 +24039,7 @@
     </row>
     <row r="736" ht="18.75" customHeight="1" spans="1:24">
       <c r="A736" s="4" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="B736" s="3"/>
       <c r="C736" s="3"/>
@@ -23944,7 +24067,7 @@
     </row>
     <row r="737" ht="18.75" customHeight="1" spans="1:24">
       <c r="A737" s="4" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="B737" s="3"/>
       <c r="C737" s="3"/>
@@ -23972,7 +24095,7 @@
     </row>
     <row r="738" ht="18.75" customHeight="1" spans="1:24">
       <c r="A738" s="4" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="B738" s="3"/>
       <c r="C738" s="3"/>
@@ -24000,7 +24123,7 @@
     </row>
     <row r="739" ht="18.75" customHeight="1" spans="1:24">
       <c r="A739" s="4" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="B739" s="3"/>
       <c r="C739" s="3"/>
@@ -24028,7 +24151,7 @@
     </row>
     <row r="740" ht="18.75" customHeight="1" spans="1:24">
       <c r="A740" s="4" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="B740" s="3"/>
       <c r="C740" s="3"/>
@@ -24056,7 +24179,7 @@
     </row>
     <row r="741" ht="18.75" customHeight="1" spans="1:24">
       <c r="A741" s="4" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="B741" s="3"/>
       <c r="C741" s="3"/>
@@ -24084,7 +24207,7 @@
     </row>
     <row r="742" ht="18.75" customHeight="1" spans="1:24">
       <c r="A742" s="4" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="B742" s="3"/>
       <c r="C742" s="3"/>
@@ -24112,7 +24235,7 @@
     </row>
     <row r="743" ht="18.75" customHeight="1" spans="1:24">
       <c r="A743" s="4" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="B743" s="3"/>
       <c r="C743" s="3"/>
@@ -24140,7 +24263,7 @@
     </row>
     <row r="744" ht="18.75" customHeight="1" spans="1:24">
       <c r="A744" s="4" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="B744" s="3"/>
       <c r="C744" s="3"/>
@@ -24168,7 +24291,7 @@
     </row>
     <row r="745" ht="18.75" customHeight="1" spans="1:24">
       <c r="A745" s="4" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="B745" s="3"/>
       <c r="C745" s="3"/>
@@ -24196,7 +24319,7 @@
     </row>
     <row r="746" ht="18.75" customHeight="1" spans="1:24">
       <c r="A746" s="4" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="B746" s="3"/>
       <c r="C746" s="3"/>
@@ -24224,7 +24347,7 @@
     </row>
     <row r="747" ht="18.75" customHeight="1" spans="1:24">
       <c r="A747" s="4" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B747" s="3"/>
       <c r="C747" s="3"/>
@@ -24252,7 +24375,7 @@
     </row>
     <row r="748" ht="18.75" customHeight="1" spans="1:24">
       <c r="A748" s="4" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="B748" s="3"/>
       <c r="C748" s="3"/>
@@ -24280,7 +24403,7 @@
     </row>
     <row r="749" ht="18.75" customHeight="1" spans="1:24">
       <c r="A749" s="4" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="B749" s="3"/>
       <c r="C749" s="3"/>
@@ -24308,7 +24431,7 @@
     </row>
     <row r="750" ht="18.75" customHeight="1" spans="1:24">
       <c r="A750" s="4" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="B750" s="3"/>
       <c r="C750" s="3"/>
@@ -24336,7 +24459,7 @@
     </row>
     <row r="751" ht="18.75" customHeight="1" spans="1:24">
       <c r="A751" s="4" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="B751" s="3"/>
       <c r="C751" s="3"/>
@@ -24364,7 +24487,7 @@
     </row>
     <row r="752" ht="18.75" customHeight="1" spans="1:24">
       <c r="A752" s="4" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="B752" s="3"/>
       <c r="C752" s="3"/>
@@ -24392,7 +24515,7 @@
     </row>
     <row r="753" ht="18.75" customHeight="1" spans="1:24">
       <c r="A753" s="4" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="B753" s="3"/>
       <c r="C753" s="3"/>
@@ -24420,7 +24543,7 @@
     </row>
     <row r="754" ht="18.75" customHeight="1" spans="1:24">
       <c r="A754" s="4" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="B754" s="3"/>
       <c r="C754" s="3"/>
@@ -24448,7 +24571,7 @@
     </row>
     <row r="755" ht="18.75" customHeight="1" spans="1:24">
       <c r="A755" s="4" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="B755" s="3"/>
       <c r="C755" s="3"/>
@@ -24476,7 +24599,7 @@
     </row>
     <row r="756" ht="18.75" customHeight="1" spans="1:24">
       <c r="A756" s="4" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="B756" s="3"/>
       <c r="C756" s="3"/>
@@ -24504,7 +24627,7 @@
     </row>
     <row r="757" ht="18.75" customHeight="1" spans="1:24">
       <c r="A757" s="4" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="B757" s="3"/>
       <c r="C757" s="3"/>
@@ -24532,7 +24655,7 @@
     </row>
     <row r="758" ht="18.75" customHeight="1" spans="1:24">
       <c r="A758" s="4" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="B758" s="3"/>
       <c r="C758" s="3"/>
@@ -24560,7 +24683,7 @@
     </row>
     <row r="759" ht="18.75" customHeight="1" spans="1:24">
       <c r="A759" s="4" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="B759" s="3"/>
       <c r="C759" s="3"/>
@@ -24588,7 +24711,7 @@
     </row>
     <row r="760" ht="18.75" customHeight="1" spans="1:24">
       <c r="A760" s="4" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B760" s="3"/>
       <c r="C760" s="3"/>
@@ -24616,7 +24739,7 @@
     </row>
     <row r="761" ht="18.75" customHeight="1" spans="1:24">
       <c r="A761" s="4" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="B761" s="3"/>
       <c r="C761" s="3"/>
@@ -24644,7 +24767,7 @@
     </row>
     <row r="762" ht="18.75" customHeight="1" spans="1:24">
       <c r="A762" s="4" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="B762" s="3"/>
       <c r="C762" s="3"/>
@@ -24672,7 +24795,7 @@
     </row>
     <row r="763" ht="18.75" customHeight="1" spans="1:24">
       <c r="A763" s="4" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="B763" s="3"/>
       <c r="C763" s="3"/>
@@ -24700,7 +24823,7 @@
     </row>
     <row r="764" ht="18.75" customHeight="1" spans="1:24">
       <c r="A764" s="4" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="B764" s="3"/>
       <c r="C764" s="3"/>
@@ -24728,7 +24851,7 @@
     </row>
     <row r="765" ht="18.75" customHeight="1" spans="1:24">
       <c r="A765" s="4" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="B765" s="3"/>
       <c r="C765" s="3"/>
@@ -24756,7 +24879,7 @@
     </row>
     <row r="766" ht="18.75" customHeight="1" spans="1:24">
       <c r="A766" s="4" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="B766" s="3"/>
       <c r="C766" s="3"/>
@@ -24784,7 +24907,7 @@
     </row>
     <row r="767" ht="18.75" customHeight="1" spans="1:24">
       <c r="A767" s="4" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="B767" s="3"/>
       <c r="C767" s="3"/>
@@ -24812,7 +24935,7 @@
     </row>
     <row r="768" ht="18.75" customHeight="1" spans="1:24">
       <c r="A768" s="4" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B768" s="3"/>
       <c r="C768" s="3"/>
@@ -24840,7 +24963,7 @@
     </row>
     <row r="769" ht="18.75" customHeight="1" spans="1:24">
       <c r="A769" s="4" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="B769" s="3"/>
       <c r="C769" s="3"/>
@@ -24868,7 +24991,7 @@
     </row>
     <row r="770" ht="18.75" customHeight="1" spans="1:24">
       <c r="A770" s="4" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="B770" s="3"/>
       <c r="C770" s="3"/>
@@ -24895,7 +25018,9 @@
       <c r="X770" s="3"/>
     </row>
     <row r="771" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A771" s="4"/>
+      <c r="A771" s="4" t="s">
+        <v>760</v>
+      </c>
       <c r="B771" s="3"/>
       <c r="C771" s="3"/>
       <c r="D771" s="3"/>
@@ -24921,7 +25046,9 @@
       <c r="X771" s="3"/>
     </row>
     <row r="772" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A772" s="4"/>
+      <c r="A772" s="4" t="s">
+        <v>761</v>
+      </c>
       <c r="B772" s="3"/>
       <c r="C772" s="3"/>
       <c r="D772" s="3"/>
@@ -24947,7 +25074,9 @@
       <c r="X772" s="3"/>
     </row>
     <row r="773" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A773" s="4"/>
+      <c r="A773" s="4" t="s">
+        <v>762</v>
+      </c>
       <c r="B773" s="3"/>
       <c r="C773" s="3"/>
       <c r="D773" s="3"/>
@@ -24973,7 +25102,9 @@
       <c r="X773" s="3"/>
     </row>
     <row r="774" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A774" s="4"/>
+      <c r="A774" s="4" t="s">
+        <v>763</v>
+      </c>
       <c r="B774" s="3"/>
       <c r="C774" s="3"/>
       <c r="D774" s="3"/>
@@ -24999,7 +25130,9 @@
       <c r="X774" s="3"/>
     </row>
     <row r="775" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A775" s="4"/>
+      <c r="A775" s="4" t="s">
+        <v>764</v>
+      </c>
       <c r="B775" s="3"/>
       <c r="C775" s="3"/>
       <c r="D775" s="3"/>
@@ -25025,7 +25158,9 @@
       <c r="X775" s="3"/>
     </row>
     <row r="776" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A776" s="4"/>
+      <c r="A776" s="4" t="s">
+        <v>765</v>
+      </c>
       <c r="B776" s="3"/>
       <c r="C776" s="3"/>
       <c r="D776" s="3"/>
@@ -25051,7 +25186,9 @@
       <c r="X776" s="3"/>
     </row>
     <row r="777" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A777" s="4"/>
+      <c r="A777" s="4" t="s">
+        <v>766</v>
+      </c>
       <c r="B777" s="3"/>
       <c r="C777" s="3"/>
       <c r="D777" s="3"/>
@@ -25077,7 +25214,9 @@
       <c r="X777" s="3"/>
     </row>
     <row r="778" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A778" s="4"/>
+      <c r="A778" s="4" t="s">
+        <v>767</v>
+      </c>
       <c r="B778" s="3"/>
       <c r="C778" s="3"/>
       <c r="D778" s="3"/>
@@ -25103,7 +25242,9 @@
       <c r="X778" s="3"/>
     </row>
     <row r="779" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A779" s="4"/>
+      <c r="A779" s="4" t="s">
+        <v>768</v>
+      </c>
       <c r="B779" s="3"/>
       <c r="C779" s="3"/>
       <c r="D779" s="3"/>
@@ -25129,7 +25270,9 @@
       <c r="X779" s="3"/>
     </row>
     <row r="780" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A780" s="4"/>
+      <c r="A780" s="4" t="s">
+        <v>769</v>
+      </c>
       <c r="B780" s="3"/>
       <c r="C780" s="3"/>
       <c r="D780" s="3"/>
@@ -25155,7 +25298,9 @@
       <c r="X780" s="3"/>
     </row>
     <row r="781" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A781" s="4"/>
+      <c r="A781" s="4" t="s">
+        <v>770</v>
+      </c>
       <c r="B781" s="3"/>
       <c r="C781" s="3"/>
       <c r="D781" s="3"/>
@@ -25181,7 +25326,9 @@
       <c r="X781" s="3"/>
     </row>
     <row r="782" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A782" s="4"/>
+      <c r="A782" s="4" t="s">
+        <v>766</v>
+      </c>
       <c r="B782" s="3"/>
       <c r="C782" s="3"/>
       <c r="D782" s="3"/>
@@ -25207,7 +25354,9 @@
       <c r="X782" s="3"/>
     </row>
     <row r="783" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A783" s="4"/>
+      <c r="A783" s="4" t="s">
+        <v>771</v>
+      </c>
       <c r="B783" s="3"/>
       <c r="C783" s="3"/>
       <c r="D783" s="3"/>
@@ -25233,7 +25382,9 @@
       <c r="X783" s="3"/>
     </row>
     <row r="784" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A784" s="4"/>
+      <c r="A784" s="4" t="s">
+        <v>772</v>
+      </c>
       <c r="B784" s="3"/>
       <c r="C784" s="3"/>
       <c r="D784" s="3"/>
@@ -25259,7 +25410,9 @@
       <c r="X784" s="3"/>
     </row>
     <row r="785" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A785" s="4"/>
+      <c r="A785" s="4" t="s">
+        <v>773</v>
+      </c>
       <c r="B785" s="3"/>
       <c r="C785" s="3"/>
       <c r="D785" s="3"/>
@@ -25285,7 +25438,9 @@
       <c r="X785" s="3"/>
     </row>
     <row r="786" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A786" s="4"/>
+      <c r="A786" s="4" t="s">
+        <v>774</v>
+      </c>
       <c r="B786" s="3"/>
       <c r="C786" s="3"/>
       <c r="D786" s="3"/>
@@ -25311,7 +25466,9 @@
       <c r="X786" s="3"/>
     </row>
     <row r="787" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A787" s="4"/>
+      <c r="A787" s="4" t="s">
+        <v>775</v>
+      </c>
       <c r="B787" s="3"/>
       <c r="C787" s="3"/>
       <c r="D787" s="3"/>
@@ -25337,7 +25494,9 @@
       <c r="X787" s="3"/>
     </row>
     <row r="788" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A788" s="4"/>
+      <c r="A788" s="4" t="s">
+        <v>776</v>
+      </c>
       <c r="B788" s="3"/>
       <c r="C788" s="3"/>
       <c r="D788" s="3"/>
@@ -25363,7 +25522,9 @@
       <c r="X788" s="3"/>
     </row>
     <row r="789" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A789" s="4"/>
+      <c r="A789" s="4" t="s">
+        <v>777</v>
+      </c>
       <c r="B789" s="3"/>
       <c r="C789" s="3"/>
       <c r="D789" s="3"/>
@@ -25389,7 +25550,9 @@
       <c r="X789" s="3"/>
     </row>
     <row r="790" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A790" s="4"/>
+      <c r="A790" s="4" t="s">
+        <v>778</v>
+      </c>
       <c r="B790" s="3"/>
       <c r="C790" s="3"/>
       <c r="D790" s="3"/>
@@ -25415,7 +25578,9 @@
       <c r="X790" s="3"/>
     </row>
     <row r="791" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A791" s="4"/>
+      <c r="A791" s="4" t="s">
+        <v>779</v>
+      </c>
       <c r="B791" s="3"/>
       <c r="C791" s="3"/>
       <c r="D791" s="3"/>
@@ -25441,7 +25606,9 @@
       <c r="X791" s="3"/>
     </row>
     <row r="792" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A792" s="4"/>
+      <c r="A792" s="4" t="s">
+        <v>780</v>
+      </c>
       <c r="B792" s="3"/>
       <c r="C792" s="3"/>
       <c r="D792" s="3"/>
@@ -25467,7 +25634,9 @@
       <c r="X792" s="3"/>
     </row>
     <row r="793" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A793" s="4"/>
+      <c r="A793" s="4" t="s">
+        <v>781</v>
+      </c>
       <c r="B793" s="3"/>
       <c r="C793" s="3"/>
       <c r="D793" s="3"/>
@@ -25493,7 +25662,9 @@
       <c r="X793" s="3"/>
     </row>
     <row r="794" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A794" s="4"/>
+      <c r="A794" s="4" t="s">
+        <v>782</v>
+      </c>
       <c r="B794" s="3"/>
       <c r="C794" s="3"/>
       <c r="D794" s="3"/>
@@ -25519,7 +25690,9 @@
       <c r="X794" s="3"/>
     </row>
     <row r="795" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A795" s="4"/>
+      <c r="A795" s="4" t="s">
+        <v>783</v>
+      </c>
       <c r="B795" s="3"/>
       <c r="C795" s="3"/>
       <c r="D795" s="3"/>
@@ -25545,7 +25718,9 @@
       <c r="X795" s="3"/>
     </row>
     <row r="796" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A796" s="4"/>
+      <c r="A796" s="4" t="s">
+        <v>784</v>
+      </c>
       <c r="B796" s="3"/>
       <c r="C796" s="3"/>
       <c r="D796" s="3"/>
@@ -25571,7 +25746,9 @@
       <c r="X796" s="3"/>
     </row>
     <row r="797" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A797" s="4"/>
+      <c r="A797" s="4" t="s">
+        <v>785</v>
+      </c>
       <c r="B797" s="3"/>
       <c r="C797" s="3"/>
       <c r="D797" s="3"/>
@@ -25597,7 +25774,9 @@
       <c r="X797" s="3"/>
     </row>
     <row r="798" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A798" s="4"/>
+      <c r="A798" s="4" t="s">
+        <v>219</v>
+      </c>
       <c r="B798" s="3"/>
       <c r="C798" s="3"/>
       <c r="D798" s="3"/>
@@ -25623,7 +25802,9 @@
       <c r="X798" s="3"/>
     </row>
     <row r="799" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A799" s="4"/>
+      <c r="A799" s="4" t="s">
+        <v>786</v>
+      </c>
       <c r="B799" s="3"/>
       <c r="C799" s="3"/>
       <c r="D799" s="3"/>
@@ -25649,7 +25830,9 @@
       <c r="X799" s="3"/>
     </row>
     <row r="800" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A800" s="4"/>
+      <c r="A800" s="4" t="s">
+        <v>787</v>
+      </c>
       <c r="B800" s="3"/>
       <c r="C800" s="3"/>
       <c r="D800" s="3"/>
@@ -25675,7 +25858,9 @@
       <c r="X800" s="3"/>
     </row>
     <row r="801" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A801" s="4"/>
+      <c r="A801" s="4" t="s">
+        <v>788</v>
+      </c>
       <c r="B801" s="3"/>
       <c r="C801" s="3"/>
       <c r="D801" s="3"/>
@@ -25701,7 +25886,9 @@
       <c r="X801" s="3"/>
     </row>
     <row r="802" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A802" s="4"/>
+      <c r="A802" s="4" t="s">
+        <v>789</v>
+      </c>
       <c r="B802" s="3"/>
       <c r="C802" s="3"/>
       <c r="D802" s="3"/>
@@ -25727,7 +25914,9 @@
       <c r="X802" s="3"/>
     </row>
     <row r="803" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A803" s="4"/>
+      <c r="A803" s="4" t="s">
+        <v>790</v>
+      </c>
       <c r="B803" s="3"/>
       <c r="C803" s="3"/>
       <c r="D803" s="3"/>
@@ -25753,7 +25942,9 @@
       <c r="X803" s="3"/>
     </row>
     <row r="804" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A804" s="4"/>
+      <c r="A804" s="4" t="s">
+        <v>791</v>
+      </c>
       <c r="B804" s="3"/>
       <c r="C804" s="3"/>
       <c r="D804" s="3"/>
@@ -25779,7 +25970,9 @@
       <c r="X804" s="3"/>
     </row>
     <row r="805" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A805" s="4"/>
+      <c r="A805" s="4" t="s">
+        <v>792</v>
+      </c>
       <c r="B805" s="3"/>
       <c r="C805" s="3"/>
       <c r="D805" s="3"/>
@@ -25805,7 +25998,9 @@
       <c r="X805" s="3"/>
     </row>
     <row r="806" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A806" s="4"/>
+      <c r="A806" s="4" t="s">
+        <v>793</v>
+      </c>
       <c r="B806" s="3"/>
       <c r="C806" s="3"/>
       <c r="D806" s="3"/>
@@ -25831,7 +26026,9 @@
       <c r="X806" s="3"/>
     </row>
     <row r="807" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A807" s="4"/>
+      <c r="A807" s="4" t="s">
+        <v>794</v>
+      </c>
       <c r="B807" s="3"/>
       <c r="C807" s="3"/>
       <c r="D807" s="3"/>
@@ -25857,7 +26054,9 @@
       <c r="X807" s="3"/>
     </row>
     <row r="808" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A808" s="4"/>
+      <c r="A808" s="4" t="s">
+        <v>795</v>
+      </c>
       <c r="B808" s="3"/>
       <c r="C808" s="3"/>
       <c r="D808" s="3"/>
@@ -25883,7 +26082,9 @@
       <c r="X808" s="3"/>
     </row>
     <row r="809" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A809" s="4"/>
+      <c r="A809" s="4" t="s">
+        <v>796</v>
+      </c>
       <c r="B809" s="3"/>
       <c r="C809" s="3"/>
       <c r="D809" s="3"/>
@@ -25909,7 +26110,9 @@
       <c r="X809" s="3"/>
     </row>
     <row r="810" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A810" s="4"/>
+      <c r="A810" s="4" t="s">
+        <v>797</v>
+      </c>
       <c r="B810" s="3"/>
       <c r="C810" s="3"/>
       <c r="D810" s="3"/>
@@ -25935,7 +26138,9 @@
       <c r="X810" s="3"/>
     </row>
     <row r="811" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A811" s="4"/>
+      <c r="A811" s="4" t="s">
+        <v>798</v>
+      </c>
       <c r="B811" s="3"/>
       <c r="C811" s="3"/>
       <c r="D811" s="3"/>
@@ -25961,7 +26166,9 @@
       <c r="X811" s="3"/>
     </row>
     <row r="812" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A812" s="4"/>
+      <c r="A812" s="4" t="s">
+        <v>799</v>
+      </c>
       <c r="B812" s="3"/>
       <c r="C812" s="3"/>
       <c r="D812" s="3"/>
@@ -27573,7 +27780,7 @@
       <c r="X873" s="3"/>
     </row>
     <row r="874" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A874" s="4"/>
+      <c r="A874" s="3"/>
       <c r="B874" s="3"/>
       <c r="C874" s="3"/>
       <c r="D874" s="3"/>
@@ -27599,7 +27806,7 @@
       <c r="X874" s="3"/>
     </row>
     <row r="875" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A875" s="4"/>
+      <c r="A875" s="3"/>
       <c r="B875" s="3"/>
       <c r="C875" s="3"/>
       <c r="D875" s="3"/>
@@ -30796,58 +31003,6 @@
       <c r="W997" s="3"/>
       <c r="X997" s="3"/>
     </row>
-    <row r="998" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A998" s="3"/>
-      <c r="B998" s="3"/>
-      <c r="C998" s="3"/>
-      <c r="D998" s="3"/>
-      <c r="E998" s="3"/>
-      <c r="F998" s="3"/>
-      <c r="G998" s="3"/>
-      <c r="H998" s="3"/>
-      <c r="I998" s="3"/>
-      <c r="J998" s="3"/>
-      <c r="K998" s="3"/>
-      <c r="L998" s="3"/>
-      <c r="M998" s="3"/>
-      <c r="N998" s="3"/>
-      <c r="O998" s="3"/>
-      <c r="P998" s="3"/>
-      <c r="Q998" s="3"/>
-      <c r="R998" s="3"/>
-      <c r="S998" s="3"/>
-      <c r="T998" s="3"/>
-      <c r="U998" s="3"/>
-      <c r="V998" s="3"/>
-      <c r="W998" s="3"/>
-      <c r="X998" s="3"/>
-    </row>
-    <row r="999" ht="18.75" customHeight="1" spans="1:24">
-      <c r="A999" s="3"/>
-      <c r="B999" s="3"/>
-      <c r="C999" s="3"/>
-      <c r="D999" s="3"/>
-      <c r="E999" s="3"/>
-      <c r="F999" s="3"/>
-      <c r="G999" s="3"/>
-      <c r="H999" s="3"/>
-      <c r="I999" s="3"/>
-      <c r="J999" s="3"/>
-      <c r="K999" s="3"/>
-      <c r="L999" s="3"/>
-      <c r="M999" s="3"/>
-      <c r="N999" s="3"/>
-      <c r="O999" s="3"/>
-      <c r="P999" s="3"/>
-      <c r="Q999" s="3"/>
-      <c r="R999" s="3"/>
-      <c r="S999" s="3"/>
-      <c r="T999" s="3"/>
-      <c r="U999" s="3"/>
-      <c r="V999" s="3"/>
-      <c r="W999" s="3"/>
-      <c r="X999" s="3"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
fix issues + 905 roots
</commit_message>
<xml_diff>
--- a/root_words.xlsx
+++ b/root_words.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="871">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="902">
   <si>
     <t>word</t>
   </si>
@@ -2627,6 +2627,99 @@
   </si>
   <si>
     <t>পানী</t>
+  </si>
+  <si>
+    <t>তৃতীয়াংশ</t>
+  </si>
+  <si>
+    <t>বহুবিস্তৃত</t>
+  </si>
+  <si>
+    <t>বিভক্ত</t>
+  </si>
+  <si>
+    <t>নানাপ্রকার</t>
+  </si>
+  <si>
+    <t>সেবামূলক</t>
+  </si>
+  <si>
+    <t>সবচেয়ে</t>
+  </si>
+  <si>
+    <t>বড়</t>
+  </si>
+  <si>
+    <t>অঙ্গরূপ</t>
+  </si>
+  <si>
+    <t>দূরীকরণ</t>
+  </si>
+  <si>
+    <t>প্রধান</t>
+  </si>
+  <si>
+    <t>দ্বিতীয়</t>
+  </si>
+  <si>
+    <t>বৃহত্তম</t>
+  </si>
+  <si>
+    <t>পল্লীসংস্কার</t>
+  </si>
+  <si>
+    <t>পল্লী</t>
+  </si>
+  <si>
+    <t>পথঘাট</t>
+  </si>
+  <si>
+    <t>নির্মাণজীর্ণ</t>
+  </si>
+  <si>
+    <t>পুকুর</t>
+  </si>
+  <si>
+    <t>সংস্কার</t>
+  </si>
+  <si>
+    <t>ব্যবস্থা</t>
+  </si>
+  <si>
+    <t>ইত্যাদি</t>
+  </si>
+  <si>
+    <t>তাছাড়া</t>
+  </si>
+  <si>
+    <t>অজ্ঞ</t>
+  </si>
+  <si>
+    <t>উদাসীন</t>
+  </si>
+  <si>
+    <t>গ্রামবাসী</t>
+  </si>
+  <si>
+    <t>স্বাস্থ্যবিধি</t>
+  </si>
+  <si>
+    <t>সচেতন</t>
+  </si>
+  <si>
+    <t>ক্ষতিকর</t>
+  </si>
+  <si>
+    <t>পরিহার</t>
+  </si>
+  <si>
+    <t>নাগরিক</t>
+  </si>
+  <si>
+    <t>দের</t>
+  </si>
+  <si>
+    <t>কর্তব্য</t>
   </si>
 </sst>
 </file>
@@ -2636,10 +2729,10 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2672,11 +2765,10 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2688,30 +2780,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2727,6 +2796,14 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -2734,7 +2811,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2749,7 +2826,59 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2765,28 +2894,6 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
@@ -2796,7 +2903,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2804,13 +2911,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2825,13 +2925,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2843,19 +2949,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2873,7 +2973,103 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2885,73 +3081,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2963,43 +3093,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3035,16 +3135,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3054,15 +3163,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3082,17 +3182,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3102,6 +3198,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3120,159 +3231,148 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3662,8 +3762,8 @@
   </sheetPr>
   <dimension ref="A1:Z995"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A863" workbookViewId="0">
-      <selection activeCell="A874" sqref="A874"/>
+    <sheetView tabSelected="1" topLeftCell="A894" workbookViewId="0">
+      <selection activeCell="A905" sqref="A905"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -10154,7 +10254,7 @@
       <c r="Y216" s="8"/>
       <c r="Z216" s="8"/>
     </row>
-    <row r="217" ht="15.75" customHeight="1" spans="1:26">
+    <row r="217" ht="21.75" customHeight="1" spans="1:26">
       <c r="A217" s="3" t="s">
         <v>216</v>
       </c>
@@ -10184,7 +10284,7 @@
       <c r="Y217" s="8"/>
       <c r="Z217" s="8"/>
     </row>
-    <row r="218" ht="15.75" customHeight="1" spans="1:26">
+    <row r="218" ht="21.75" customHeight="1" spans="1:26">
       <c r="A218" s="3" t="s">
         <v>217</v>
       </c>
@@ -10214,7 +10314,7 @@
       <c r="Y218" s="8"/>
       <c r="Z218" s="8"/>
     </row>
-    <row r="219" ht="15.75" customHeight="1" spans="1:26">
+    <row r="219" ht="21.75" customHeight="1" spans="1:26">
       <c r="A219" s="3" t="s">
         <v>218</v>
       </c>
@@ -10244,7 +10344,7 @@
       <c r="Y219" s="8"/>
       <c r="Z219" s="8"/>
     </row>
-    <row r="220" ht="15.75" customHeight="1" spans="1:26">
+    <row r="220" ht="21.75" customHeight="1" spans="1:26">
       <c r="A220" s="3" t="s">
         <v>219</v>
       </c>
@@ -29894,7 +29994,10 @@
       <c r="Y874" s="8"/>
       <c r="Z874" s="8"/>
     </row>
-    <row r="875" ht="15.75" customHeight="1" spans="2:26">
+    <row r="875" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A875" s="1" t="s">
+        <v>871</v>
+      </c>
       <c r="B875" s="4"/>
       <c r="C875" s="4"/>
       <c r="D875" s="4"/>
@@ -29921,7 +30024,10 @@
       <c r="Y875" s="8"/>
       <c r="Z875" s="8"/>
     </row>
-    <row r="876" ht="15.75" customHeight="1" spans="2:26">
+    <row r="876" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A876" s="1" t="s">
+        <v>872</v>
+      </c>
       <c r="B876" s="4"/>
       <c r="C876" s="4"/>
       <c r="D876" s="4"/>
@@ -29948,7 +30054,10 @@
       <c r="Y876" s="8"/>
       <c r="Z876" s="8"/>
     </row>
-    <row r="877" ht="15.75" customHeight="1" spans="2:26">
+    <row r="877" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A877" s="1" t="s">
+        <v>873</v>
+      </c>
       <c r="B877" s="4"/>
       <c r="C877" s="4"/>
       <c r="D877" s="4"/>
@@ -29975,7 +30084,10 @@
       <c r="Y877" s="8"/>
       <c r="Z877" s="8"/>
     </row>
-    <row r="878" ht="15.75" customHeight="1" spans="2:26">
+    <row r="878" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A878" s="1" t="s">
+        <v>874</v>
+      </c>
       <c r="B878" s="4"/>
       <c r="C878" s="4"/>
       <c r="D878" s="4"/>
@@ -30002,7 +30114,10 @@
       <c r="Y878" s="8"/>
       <c r="Z878" s="8"/>
     </row>
-    <row r="879" ht="15.75" customHeight="1" spans="2:26">
+    <row r="879" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A879" s="1" t="s">
+        <v>875</v>
+      </c>
       <c r="B879" s="4"/>
       <c r="C879" s="4"/>
       <c r="D879" s="4"/>
@@ -30029,7 +30144,10 @@
       <c r="Y879" s="8"/>
       <c r="Z879" s="8"/>
     </row>
-    <row r="880" ht="15.75" customHeight="1" spans="2:26">
+    <row r="880" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A880" s="1" t="s">
+        <v>876</v>
+      </c>
       <c r="B880" s="4"/>
       <c r="C880" s="4"/>
       <c r="D880" s="4"/>
@@ -30056,7 +30174,10 @@
       <c r="Y880" s="8"/>
       <c r="Z880" s="8"/>
     </row>
-    <row r="881" ht="15.75" customHeight="1" spans="2:26">
+    <row r="881" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A881" s="1" t="s">
+        <v>877</v>
+      </c>
       <c r="B881" s="4"/>
       <c r="C881" s="4"/>
       <c r="D881" s="4"/>
@@ -30083,7 +30204,10 @@
       <c r="Y881" s="8"/>
       <c r="Z881" s="8"/>
     </row>
-    <row r="882" ht="15.75" customHeight="1" spans="2:26">
+    <row r="882" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A882" s="1" t="s">
+        <v>878</v>
+      </c>
       <c r="B882" s="4"/>
       <c r="C882" s="4"/>
       <c r="D882" s="4"/>
@@ -30110,7 +30234,10 @@
       <c r="Y882" s="8"/>
       <c r="Z882" s="8"/>
     </row>
-    <row r="883" ht="15.75" customHeight="1" spans="2:26">
+    <row r="883" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A883" s="1" t="s">
+        <v>879</v>
+      </c>
       <c r="B883" s="4"/>
       <c r="C883" s="4"/>
       <c r="D883" s="4"/>
@@ -30137,7 +30264,10 @@
       <c r="Y883" s="8"/>
       <c r="Z883" s="8"/>
     </row>
-    <row r="884" ht="15.75" customHeight="1" spans="2:26">
+    <row r="884" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A884" s="1" t="s">
+        <v>880</v>
+      </c>
       <c r="B884" s="4"/>
       <c r="C884" s="4"/>
       <c r="D884" s="4"/>
@@ -30164,7 +30294,10 @@
       <c r="Y884" s="8"/>
       <c r="Z884" s="8"/>
     </row>
-    <row r="885" ht="15.75" customHeight="1" spans="2:26">
+    <row r="885" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A885" s="1" t="s">
+        <v>881</v>
+      </c>
       <c r="B885" s="4"/>
       <c r="C885" s="4"/>
       <c r="D885" s="4"/>
@@ -30191,7 +30324,10 @@
       <c r="Y885" s="8"/>
       <c r="Z885" s="8"/>
     </row>
-    <row r="886" ht="15.75" customHeight="1" spans="2:26">
+    <row r="886" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A886" s="1" t="s">
+        <v>882</v>
+      </c>
       <c r="B886" s="4"/>
       <c r="C886" s="4"/>
       <c r="D886" s="4"/>
@@ -30218,7 +30354,10 @@
       <c r="Y886" s="8"/>
       <c r="Z886" s="8"/>
     </row>
-    <row r="887" ht="15.75" customHeight="1" spans="2:26">
+    <row r="887" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A887" s="1" t="s">
+        <v>883</v>
+      </c>
       <c r="B887" s="4"/>
       <c r="C887" s="4"/>
       <c r="D887" s="4"/>
@@ -30245,7 +30384,10 @@
       <c r="Y887" s="8"/>
       <c r="Z887" s="8"/>
     </row>
-    <row r="888" ht="15.75" customHeight="1" spans="2:26">
+    <row r="888" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A888" s="1" t="s">
+        <v>884</v>
+      </c>
       <c r="B888" s="4"/>
       <c r="C888" s="4"/>
       <c r="D888" s="4"/>
@@ -30272,7 +30414,10 @@
       <c r="Y888" s="8"/>
       <c r="Z888" s="8"/>
     </row>
-    <row r="889" ht="15.75" customHeight="1" spans="2:26">
+    <row r="889" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A889" s="1" t="s">
+        <v>885</v>
+      </c>
       <c r="B889" s="4"/>
       <c r="C889" s="4"/>
       <c r="D889" s="4"/>
@@ -30299,7 +30444,10 @@
       <c r="Y889" s="8"/>
       <c r="Z889" s="8"/>
     </row>
-    <row r="890" ht="15.75" customHeight="1" spans="2:26">
+    <row r="890" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A890" s="1" t="s">
+        <v>886</v>
+      </c>
       <c r="B890" s="4"/>
       <c r="C890" s="4"/>
       <c r="D890" s="4"/>
@@ -30326,7 +30474,10 @@
       <c r="Y890" s="8"/>
       <c r="Z890" s="8"/>
     </row>
-    <row r="891" ht="15.75" customHeight="1" spans="2:26">
+    <row r="891" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A891" s="1" t="s">
+        <v>887</v>
+      </c>
       <c r="B891" s="4"/>
       <c r="C891" s="4"/>
       <c r="D891" s="4"/>
@@ -30353,7 +30504,10 @@
       <c r="Y891" s="8"/>
       <c r="Z891" s="8"/>
     </row>
-    <row r="892" ht="15.75" customHeight="1" spans="2:26">
+    <row r="892" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A892" s="1" t="s">
+        <v>888</v>
+      </c>
       <c r="B892" s="4"/>
       <c r="C892" s="4"/>
       <c r="D892" s="4"/>
@@ -30380,7 +30534,10 @@
       <c r="Y892" s="8"/>
       <c r="Z892" s="8"/>
     </row>
-    <row r="893" ht="15.75" customHeight="1" spans="2:26">
+    <row r="893" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A893" s="1" t="s">
+        <v>889</v>
+      </c>
       <c r="B893" s="4"/>
       <c r="C893" s="4"/>
       <c r="D893" s="4"/>
@@ -30407,7 +30564,10 @@
       <c r="Y893" s="8"/>
       <c r="Z893" s="8"/>
     </row>
-    <row r="894" ht="15.75" customHeight="1" spans="2:26">
+    <row r="894" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A894" s="1" t="s">
+        <v>890</v>
+      </c>
       <c r="B894" s="4"/>
       <c r="C894" s="4"/>
       <c r="D894" s="4"/>
@@ -30434,7 +30594,10 @@
       <c r="Y894" s="8"/>
       <c r="Z894" s="8"/>
     </row>
-    <row r="895" ht="15.75" customHeight="1" spans="2:26">
+    <row r="895" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A895" s="1" t="s">
+        <v>891</v>
+      </c>
       <c r="B895" s="4"/>
       <c r="C895" s="4"/>
       <c r="D895" s="4"/>
@@ -30461,7 +30624,10 @@
       <c r="Y895" s="8"/>
       <c r="Z895" s="8"/>
     </row>
-    <row r="896" ht="15.75" customHeight="1" spans="2:26">
+    <row r="896" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A896" s="1" t="s">
+        <v>892</v>
+      </c>
       <c r="B896" s="4"/>
       <c r="C896" s="4"/>
       <c r="D896" s="4"/>
@@ -30488,7 +30654,10 @@
       <c r="Y896" s="8"/>
       <c r="Z896" s="8"/>
     </row>
-    <row r="897" ht="15.75" customHeight="1" spans="2:26">
+    <row r="897" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A897" s="1" t="s">
+        <v>893</v>
+      </c>
       <c r="B897" s="4"/>
       <c r="C897" s="4"/>
       <c r="D897" s="4"/>
@@ -30515,7 +30684,10 @@
       <c r="Y897" s="8"/>
       <c r="Z897" s="8"/>
     </row>
-    <row r="898" ht="15.75" customHeight="1" spans="2:26">
+    <row r="898" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A898" s="1" t="s">
+        <v>894</v>
+      </c>
       <c r="B898" s="8"/>
       <c r="C898" s="8"/>
       <c r="D898" s="8"/>
@@ -30542,7 +30714,10 @@
       <c r="Y898" s="8"/>
       <c r="Z898" s="8"/>
     </row>
-    <row r="899" ht="15.75" customHeight="1" spans="2:26">
+    <row r="899" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A899" s="1" t="s">
+        <v>895</v>
+      </c>
       <c r="B899" s="8"/>
       <c r="C899" s="8"/>
       <c r="D899" s="8"/>
@@ -30569,7 +30744,10 @@
       <c r="Y899" s="8"/>
       <c r="Z899" s="8"/>
     </row>
-    <row r="900" ht="15.75" customHeight="1" spans="2:26">
+    <row r="900" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A900" s="1" t="s">
+        <v>896</v>
+      </c>
       <c r="B900" s="8"/>
       <c r="C900" s="8"/>
       <c r="D900" s="8"/>
@@ -30596,7 +30774,10 @@
       <c r="Y900" s="8"/>
       <c r="Z900" s="8"/>
     </row>
-    <row r="901" ht="15.75" customHeight="1" spans="2:26">
+    <row r="901" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A901" s="1" t="s">
+        <v>897</v>
+      </c>
       <c r="B901" s="8"/>
       <c r="C901" s="8"/>
       <c r="D901" s="8"/>
@@ -30623,7 +30804,10 @@
       <c r="Y901" s="8"/>
       <c r="Z901" s="8"/>
     </row>
-    <row r="902" ht="15.75" customHeight="1" spans="2:26">
+    <row r="902" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A902" s="1" t="s">
+        <v>898</v>
+      </c>
       <c r="B902" s="8"/>
       <c r="C902" s="8"/>
       <c r="D902" s="8"/>
@@ -30650,7 +30834,10 @@
       <c r="Y902" s="8"/>
       <c r="Z902" s="8"/>
     </row>
-    <row r="903" ht="15.75" customHeight="1" spans="2:26">
+    <row r="903" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A903" s="1" t="s">
+        <v>899</v>
+      </c>
       <c r="B903" s="8"/>
       <c r="C903" s="8"/>
       <c r="D903" s="8"/>
@@ -30677,7 +30864,10 @@
       <c r="Y903" s="8"/>
       <c r="Z903" s="8"/>
     </row>
-    <row r="904" ht="15.75" customHeight="1" spans="2:26">
+    <row r="904" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A904" s="1" t="s">
+        <v>900</v>
+      </c>
       <c r="B904" s="8"/>
       <c r="C904" s="8"/>
       <c r="D904" s="8"/>
@@ -30704,7 +30894,10 @@
       <c r="Y904" s="8"/>
       <c r="Z904" s="8"/>
     </row>
-    <row r="905" ht="15.75" customHeight="1" spans="2:26">
+    <row r="905" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A905" s="1" t="s">
+        <v>901</v>
+      </c>
       <c r="B905" s="8"/>
       <c r="C905" s="8"/>
       <c r="D905" s="8"/>

</xml_diff>

<commit_message>
add dataset more than 1000
</commit_message>
<xml_diff>
--- a/root_words.xlsx
+++ b/root_words.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215"/>
+    <workbookView windowWidth="11520" windowHeight="9072"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="905" uniqueCount="902">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="1015">
   <si>
     <t>word</t>
   </si>
@@ -235,9 +235,6 @@
     <t>আমি</t>
   </si>
   <si>
-    <t>আরও</t>
-  </si>
-  <si>
     <t>আরম্ভ</t>
   </si>
   <si>
@@ -1969,7 +1966,7 @@
     <t>যুবক</t>
   </si>
   <si>
-    <t>যে</t>
+    <t>যা</t>
   </si>
   <si>
     <t>যেকোনো</t>
@@ -2720,6 +2717,349 @@
   </si>
   <si>
     <t>কর্তব্য</t>
+  </si>
+  <si>
+    <t>পাটি</t>
+  </si>
+  <si>
+    <t>ভাঙা</t>
+  </si>
+  <si>
+    <t>হাতঘড়ি</t>
+  </si>
+  <si>
+    <t>কফি</t>
+  </si>
+  <si>
+    <t>আঁকা</t>
+  </si>
+  <si>
+    <t>মেশিন</t>
+  </si>
+  <si>
+    <t>ছবি</t>
+  </si>
+  <si>
+    <t>চাবি</t>
+  </si>
+  <si>
+    <t>অজানা</t>
+  </si>
+  <si>
+    <t>জড়ানো</t>
+  </si>
+  <si>
+    <t>তুচ্ছ</t>
+  </si>
+  <si>
+    <t>জিনিস</t>
+  </si>
+  <si>
+    <t>সুমন্ত্র</t>
+  </si>
+  <si>
+    <t>চট্টোপাধ্যায়</t>
+  </si>
+  <si>
+    <t>কুড়ুল</t>
+  </si>
+  <si>
+    <t>ধ্বংসলীল</t>
+  </si>
+  <si>
+    <t>উচিত</t>
+  </si>
+  <si>
+    <t>জাদুঘর</t>
+  </si>
+  <si>
+    <t>ঠিকঠাক</t>
+  </si>
+  <si>
+    <t>ঠিক</t>
+  </si>
+  <si>
+    <t>সকাল</t>
+  </si>
+  <si>
+    <t>আর</t>
+  </si>
+  <si>
+    <t>ব্যাগপত্র</t>
+  </si>
+  <si>
+    <t>গোছানো</t>
+  </si>
+  <si>
+    <t>বাড়ি</t>
+  </si>
+  <si>
+    <t>আসবাব</t>
+  </si>
+  <si>
+    <t>কেনা</t>
+  </si>
+  <si>
+    <t>কত</t>
+  </si>
+  <si>
+    <t>সেখান</t>
+  </si>
+  <si>
+    <t>পাতা</t>
+  </si>
+  <si>
+    <t>নেওয়া</t>
+  </si>
+  <si>
+    <t>ফালাফালা</t>
+  </si>
+  <si>
+    <t>ফালা</t>
+  </si>
+  <si>
+    <t>কয়েকদিন</t>
+  </si>
+  <si>
+    <t>নাকি</t>
+  </si>
+  <si>
+    <t>সমস্ত</t>
+  </si>
+  <si>
+    <t>সযত্ন</t>
+  </si>
+  <si>
+    <t>মিউজিইয়াম</t>
+  </si>
+  <si>
+    <t>ব্রোকেন</t>
+  </si>
+  <si>
+    <t>রিলেশনশিপ</t>
+  </si>
+  <si>
+    <t>শোভা</t>
+  </si>
+  <si>
+    <t>পাওয়া</t>
+  </si>
+  <si>
+    <t>অ্যাড্রিয়াটিক</t>
+  </si>
+  <si>
+    <t>সমুদ্রতীর</t>
+  </si>
+  <si>
+    <t>দক্ষিণ</t>
+  </si>
+  <si>
+    <t>পূর্ব</t>
+  </si>
+  <si>
+    <t>ইউরোপ</t>
+  </si>
+  <si>
+    <t>সংযোগস্থল</t>
+  </si>
+  <si>
+    <t>অবস্থিত</t>
+  </si>
+  <si>
+    <t>ক্রোয়েশিয়া</t>
+  </si>
+  <si>
+    <t>রাজধানী</t>
+  </si>
+  <si>
+    <t>জাগ্রেব</t>
+  </si>
+  <si>
+    <t>ঠিকানা</t>
+  </si>
+  <si>
+    <t>চলচ্চিত্র</t>
+  </si>
+  <si>
+    <t>প্রযোজক</t>
+  </si>
+  <si>
+    <t>ওলিঙ্কা</t>
+  </si>
+  <si>
+    <t>ভিসটিকা
+ভাস্কর</t>
+  </si>
+  <si>
+    <t>গ্রুবিসিক</t>
+  </si>
+  <si>
+    <t>দ্রাজেন</t>
+  </si>
+  <si>
+    <t>ভাস্কর</t>
+  </si>
+  <si>
+    <t>বিচ্ছেদ</t>
+  </si>
+  <si>
+    <t>বেদনা</t>
+  </si>
+  <si>
+    <t>তাঁরা</t>
+  </si>
+  <si>
+    <t>বর</t>
+  </si>
+  <si>
+    <t>বিয়ে</t>
+  </si>
+  <si>
+    <t>জড়ানো</t>
+  </si>
+  <si>
+    <t>জিনিসপত্র</t>
+  </si>
+  <si>
+    <t>সংগ্রহ</t>
+  </si>
+  <si>
+    <t>বেশ</t>
+  </si>
+  <si>
+    <t>গোড়া</t>
+  </si>
+  <si>
+    <t>ছিল</t>
+  </si>
+  <si>
+    <t>নেহাত</t>
+  </si>
+  <si>
+    <t>নড়াচড়া</t>
+  </si>
+  <si>
+    <t>দুজন</t>
+  </si>
+  <si>
+    <t>এমন</t>
+  </si>
+  <si>
+    <t>জোটা</t>
+  </si>
+  <si>
+    <t>প্রদর্শন</t>
+  </si>
+  <si>
+    <t>জাগ্রেবের</t>
+  </si>
+  <si>
+    <t>আর্ট</t>
+  </si>
+  <si>
+    <t>গ্যালারি</t>
+  </si>
+  <si>
+    <t>ভ্রমণ</t>
+  </si>
+  <si>
+    <t>জার্মানি</t>
+  </si>
+  <si>
+    <t>বসনিয়া</t>
+  </si>
+  <si>
+    <t>আর্জেন্টিনা</t>
+  </si>
+  <si>
+    <t>আফ্রিকা</t>
+  </si>
+  <si>
+    <t>সিঙ্গাপুর</t>
+  </si>
+  <si>
+    <t>তুরস্ক</t>
+  </si>
+  <si>
+    <t>আমেরিকা</t>
+  </si>
+  <si>
+    <t>সমব্যথা</t>
+  </si>
+  <si>
+    <t>দান</t>
+  </si>
+  <si>
+    <t>বাড়া</t>
+  </si>
+  <si>
+    <t>সম্ভার</t>
+  </si>
+  <si>
+    <t>বার্লিন</t>
+  </si>
+  <si>
+    <t>টি</t>
+  </si>
+  <si>
+    <t>নতুন</t>
+  </si>
+  <si>
+    <t>মাখা</t>
+  </si>
+  <si>
+    <t>মন্ত্র</t>
+  </si>
+  <si>
+    <t>কয়েকবার</t>
+  </si>
+  <si>
+    <t>কয়েক</t>
+  </si>
+  <si>
+    <t>বারবার</t>
+  </si>
+  <si>
+    <t>আবেদন</t>
+  </si>
+  <si>
+    <t>প্রতি</t>
+  </si>
+  <si>
+    <t>প্রতিবার</t>
+  </si>
+  <si>
+    <t>বার</t>
+  </si>
+  <si>
+    <t>ব্যর্থ</t>
+  </si>
+  <si>
+    <t>রোখ</t>
+  </si>
+  <si>
+    <t>চাপা</t>
+  </si>
+  <si>
+    <t>গোলগোল</t>
+  </si>
+  <si>
+    <t>গোল</t>
+  </si>
+  <si>
+    <t>বর্গফুট</t>
+  </si>
+  <si>
+    <t>জায়গা</t>
+  </si>
+  <si>
+    <t>বাস্তব</t>
+  </si>
+  <si>
+    <t>সংগ্রহশালা</t>
+  </si>
+  <si>
+    <t>অব</t>
   </si>
 </sst>
 </file>
@@ -2728,11 +3068,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2768,7 +3108,15 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2779,18 +3127,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2810,6 +3158,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -2818,31 +3174,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2856,29 +3188,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2901,9 +3212,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2925,7 +3258,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2937,175 +3438,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3130,39 +3463,6 @@
       </top>
       <bottom style="medium">
         <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3196,8 +3496,56 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3216,170 +3564,155 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3411,6 +3744,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -3760,10 +4096,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z1022"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A894" workbookViewId="0">
-      <selection activeCell="A905" sqref="A905"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" topLeftCell="A1007" workbookViewId="0">
+      <selection activeCell="A1023" sqref="A1023"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -5965,7 +6301,7 @@
       <c r="Z73" s="8"/>
     </row>
     <row r="74" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A74" s="3" t="s">
+      <c r="A74" s="7" t="s">
         <v>73</v>
       </c>
       <c r="B74" s="3"/>
@@ -5995,7 +6331,7 @@
       <c r="Z74" s="8"/>
     </row>
     <row r="75" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="3" t="s">
         <v>74</v>
       </c>
       <c r="B75" s="3"/>
@@ -6475,7 +6811,7 @@
       <c r="Z90" s="8"/>
     </row>
     <row r="91" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A91" s="3" t="s">
+      <c r="A91" s="6" t="s">
         <v>90</v>
       </c>
       <c r="B91" s="3"/>
@@ -6505,7 +6841,7 @@
       <c r="Z91" s="8"/>
     </row>
     <row r="92" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A92" s="6" t="s">
+      <c r="A92" s="3" t="s">
         <v>91</v>
       </c>
       <c r="B92" s="3"/>
@@ -6925,7 +7261,7 @@
       <c r="Z105" s="8"/>
     </row>
     <row r="106" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A106" s="3" t="s">
+      <c r="A106" s="5" t="s">
         <v>105</v>
       </c>
       <c r="B106" s="3"/>
@@ -6955,7 +7291,7 @@
       <c r="Z106" s="8"/>
     </row>
     <row r="107" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A107" s="5" t="s">
+      <c r="A107" s="3" t="s">
         <v>106</v>
       </c>
       <c r="B107" s="3"/>
@@ -7705,7 +8041,7 @@
       <c r="Z131" s="8"/>
     </row>
     <row r="132" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A132" s="3" t="s">
+      <c r="A132" s="6" t="s">
         <v>131</v>
       </c>
       <c r="B132" s="3"/>
@@ -7735,7 +8071,7 @@
       <c r="Z132" s="8"/>
     </row>
     <row r="133" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A133" s="6" t="s">
+      <c r="A133" s="3" t="s">
         <v>132</v>
       </c>
       <c r="B133" s="3"/>
@@ -8185,7 +8521,7 @@
       <c r="Z147" s="8"/>
     </row>
     <row r="148" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A148" s="3" t="s">
+      <c r="A148" s="7" t="s">
         <v>147</v>
       </c>
       <c r="B148" s="3"/>
@@ -8215,7 +8551,7 @@
       <c r="Z148" s="8"/>
     </row>
     <row r="149" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A149" s="7" t="s">
+      <c r="A149" s="3" t="s">
         <v>148</v>
       </c>
       <c r="B149" s="3"/>
@@ -10224,7 +10560,7 @@
       <c r="Y215" s="8"/>
       <c r="Z215" s="8"/>
     </row>
-    <row r="216" ht="15.75" customHeight="1" spans="1:26">
+    <row r="216" ht="21.75" customHeight="1" spans="1:26">
       <c r="A216" s="3" t="s">
         <v>215</v>
       </c>
@@ -10974,7 +11310,7 @@
       <c r="Y240" s="8"/>
       <c r="Z240" s="8"/>
     </row>
-    <row r="241" ht="21.75" customHeight="1" spans="1:26">
+    <row r="241" ht="15.75" customHeight="1" spans="1:26">
       <c r="A241" s="3" t="s">
         <v>240</v>
       </c>
@@ -11395,7 +11731,7 @@
       <c r="Z254" s="8"/>
     </row>
     <row r="255" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A255" s="3" t="s">
+      <c r="A255" s="6" t="s">
         <v>254</v>
       </c>
       <c r="B255" s="3"/>
@@ -11425,7 +11761,7 @@
       <c r="Z255" s="8"/>
     </row>
     <row r="256" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A256" s="6" t="s">
+      <c r="A256" s="3" t="s">
         <v>255</v>
       </c>
       <c r="B256" s="3"/>
@@ -11995,7 +12331,7 @@
       <c r="Z274" s="8"/>
     </row>
     <row r="275" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A275" s="3" t="s">
+      <c r="A275" s="7" t="s">
         <v>274</v>
       </c>
       <c r="B275" s="3"/>
@@ -12025,7 +12361,7 @@
       <c r="Z275" s="8"/>
     </row>
     <row r="276" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A276" s="7" t="s">
+      <c r="A276" s="3" t="s">
         <v>275</v>
       </c>
       <c r="B276" s="3"/>
@@ -12745,7 +13081,7 @@
       <c r="Z299" s="8"/>
     </row>
     <row r="300" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A300" s="3" t="s">
+      <c r="A300" s="6" t="s">
         <v>299</v>
       </c>
       <c r="B300" s="3"/>
@@ -12775,7 +13111,7 @@
       <c r="Z300" s="8"/>
     </row>
     <row r="301" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A301" s="6" t="s">
+      <c r="A301" s="3" t="s">
         <v>300</v>
       </c>
       <c r="B301" s="3"/>
@@ -13555,7 +13891,7 @@
       <c r="Z326" s="8"/>
     </row>
     <row r="327" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A327" s="3" t="s">
+      <c r="A327" s="7" t="s">
         <v>326</v>
       </c>
       <c r="B327" s="3"/>
@@ -13585,7 +13921,7 @@
       <c r="Z327" s="8"/>
     </row>
     <row r="328" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A328" s="7" t="s">
+      <c r="A328" s="3" t="s">
         <v>327</v>
       </c>
       <c r="B328" s="3"/>
@@ -13705,7 +14041,7 @@
       <c r="Z331" s="8"/>
     </row>
     <row r="332" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A332" s="3" t="s">
+      <c r="A332" s="6" t="s">
         <v>331</v>
       </c>
       <c r="B332" s="3"/>
@@ -13735,7 +14071,7 @@
       <c r="Z332" s="8"/>
     </row>
     <row r="333" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A333" s="6" t="s">
+      <c r="A333" s="3" t="s">
         <v>332</v>
       </c>
       <c r="B333" s="3"/>
@@ -14125,7 +14461,7 @@
       <c r="Z345" s="8"/>
     </row>
     <row r="346" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A346" s="3" t="s">
+      <c r="A346" s="6" t="s">
         <v>345</v>
       </c>
       <c r="B346" s="3"/>
@@ -14155,7 +14491,7 @@
       <c r="Z346" s="8"/>
     </row>
     <row r="347" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A347" s="6" t="s">
+      <c r="A347" s="3" t="s">
         <v>346</v>
       </c>
       <c r="B347" s="3"/>
@@ -14245,7 +14581,7 @@
       <c r="Z349" s="8"/>
     </row>
     <row r="350" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A350" s="3" t="s">
+      <c r="A350" s="6" t="s">
         <v>349</v>
       </c>
       <c r="B350" s="3"/>
@@ -14275,7 +14611,7 @@
       <c r="Z350" s="8"/>
     </row>
     <row r="351" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A351" s="6" t="s">
+      <c r="A351" s="3" t="s">
         <v>350</v>
       </c>
       <c r="B351" s="3"/>
@@ -14935,7 +15271,7 @@
       <c r="Z372" s="8"/>
     </row>
     <row r="373" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A373" s="3" t="s">
+      <c r="A373" s="5" t="s">
         <v>372</v>
       </c>
       <c r="B373" s="3"/>
@@ -14965,7 +15301,7 @@
       <c r="Z373" s="8"/>
     </row>
     <row r="374" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A374" s="5" t="s">
+      <c r="A374" s="3" t="s">
         <v>373</v>
       </c>
       <c r="B374" s="3"/>
@@ -14995,7 +15331,7 @@
       <c r="Z374" s="8"/>
     </row>
     <row r="375" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A375" s="3" t="s">
+      <c r="A375" s="6" t="s">
         <v>374</v>
       </c>
       <c r="B375" s="3"/>
@@ -15025,7 +15361,7 @@
       <c r="Z375" s="8"/>
     </row>
     <row r="376" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A376" s="6" t="s">
+      <c r="A376" s="3" t="s">
         <v>375</v>
       </c>
       <c r="B376" s="3"/>
@@ -15235,7 +15571,7 @@
       <c r="Z382" s="8"/>
     </row>
     <row r="383" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A383" s="3" t="s">
+      <c r="A383" s="6" t="s">
         <v>382</v>
       </c>
       <c r="B383" s="3"/>
@@ -15265,7 +15601,7 @@
       <c r="Z383" s="8"/>
     </row>
     <row r="384" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A384" s="6" t="s">
+      <c r="A384" s="3" t="s">
         <v>383</v>
       </c>
       <c r="B384" s="3"/>
@@ -15925,7 +16261,7 @@
       <c r="Z405" s="8"/>
     </row>
     <row r="406" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A406" s="3" t="s">
+      <c r="A406" s="7" t="s">
         <v>405</v>
       </c>
       <c r="B406" s="3"/>
@@ -15955,7 +16291,7 @@
       <c r="Z406" s="8"/>
     </row>
     <row r="407" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A407" s="7" t="s">
+      <c r="A407" s="3" t="s">
         <v>406</v>
       </c>
       <c r="B407" s="3"/>
@@ -16135,7 +16471,7 @@
       <c r="Z412" s="8"/>
     </row>
     <row r="413" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A413" s="3" t="s">
+      <c r="A413" s="7" t="s">
         <v>412</v>
       </c>
       <c r="B413" s="3"/>
@@ -16165,7 +16501,7 @@
       <c r="Z413" s="8"/>
     </row>
     <row r="414" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A414" s="7" t="s">
+      <c r="A414" s="5" t="s">
         <v>413</v>
       </c>
       <c r="B414" s="3"/>
@@ -16195,7 +16531,7 @@
       <c r="Z414" s="8"/>
     </row>
     <row r="415" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A415" s="5" t="s">
+      <c r="A415" s="3" t="s">
         <v>414</v>
       </c>
       <c r="B415" s="3"/>
@@ -17005,7 +17341,7 @@
       <c r="Z441" s="8"/>
     </row>
     <row r="442" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A442" s="3" t="s">
+      <c r="A442" s="5" t="s">
         <v>441</v>
       </c>
       <c r="B442" s="3"/>
@@ -17035,7 +17371,7 @@
       <c r="Z442" s="8"/>
     </row>
     <row r="443" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A443" s="5" t="s">
+      <c r="A443" s="3" t="s">
         <v>442</v>
       </c>
       <c r="B443" s="3"/>
@@ -17425,7 +17761,7 @@
       <c r="Z455" s="8"/>
     </row>
     <row r="456" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A456" s="3" t="s">
+      <c r="A456" s="6" t="s">
         <v>455</v>
       </c>
       <c r="B456" s="3"/>
@@ -17455,7 +17791,7 @@
       <c r="Z456" s="8"/>
     </row>
     <row r="457" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A457" s="6" t="s">
+      <c r="A457" s="3" t="s">
         <v>456</v>
       </c>
       <c r="B457" s="3"/>
@@ -18205,7 +18541,7 @@
       <c r="Z481" s="8"/>
     </row>
     <row r="482" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A482" s="3" t="s">
+      <c r="A482" s="5" t="s">
         <v>481</v>
       </c>
       <c r="B482" s="3"/>
@@ -18235,7 +18571,7 @@
       <c r="Z482" s="8"/>
     </row>
     <row r="483" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A483" s="5" t="s">
+      <c r="A483" s="3" t="s">
         <v>482</v>
       </c>
       <c r="B483" s="3"/>
@@ -20155,7 +20491,7 @@
       <c r="Z546" s="8"/>
     </row>
     <row r="547" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A547" s="3" t="s">
+      <c r="A547" s="6" t="s">
         <v>546</v>
       </c>
       <c r="B547" s="3"/>
@@ -20185,7 +20521,7 @@
       <c r="Z547" s="8"/>
     </row>
     <row r="548" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A548" s="6" t="s">
+      <c r="A548" s="3" t="s">
         <v>547</v>
       </c>
       <c r="B548" s="3"/>
@@ -20785,7 +21121,7 @@
       <c r="Z567" s="8"/>
     </row>
     <row r="568" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A568" s="3" t="s">
+      <c r="A568" s="9" t="s">
         <v>567</v>
       </c>
       <c r="B568" s="3"/>
@@ -20845,7 +21181,7 @@
       <c r="Z569" s="8"/>
     </row>
     <row r="570" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A570" s="9" t="s">
+      <c r="A570" s="7" t="s">
         <v>569</v>
       </c>
       <c r="B570" s="3"/>
@@ -20875,7 +21211,7 @@
       <c r="Z570" s="8"/>
     </row>
     <row r="571" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A571" s="7" t="s">
+      <c r="A571" s="3" t="s">
         <v>570</v>
       </c>
       <c r="B571" s="3"/>
@@ -21055,7 +21391,7 @@
       <c r="Z576" s="8"/>
     </row>
     <row r="577" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A577" s="3" t="s">
+      <c r="A577" s="9" t="s">
         <v>576</v>
       </c>
       <c r="B577" s="3"/>
@@ -21085,7 +21421,7 @@
       <c r="Z577" s="8"/>
     </row>
     <row r="578" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A578" s="9" t="s">
+      <c r="A578" s="3" t="s">
         <v>577</v>
       </c>
       <c r="B578" s="3"/>
@@ -21205,7 +21541,7 @@
       <c r="Z581" s="8"/>
     </row>
     <row r="582" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A582" s="3" t="s">
+      <c r="A582" s="9" t="s">
         <v>581</v>
       </c>
       <c r="B582" s="3"/>
@@ -21235,7 +21571,7 @@
       <c r="Z582" s="8"/>
     </row>
     <row r="583" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A583" s="9" t="s">
+      <c r="A583" s="3" t="s">
         <v>582</v>
       </c>
       <c r="B583" s="3"/>
@@ -21475,7 +21811,7 @@
       <c r="Z590" s="8"/>
     </row>
     <row r="591" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A591" s="3" t="s">
+      <c r="A591" s="9" t="s">
         <v>590</v>
       </c>
       <c r="B591" s="3"/>
@@ -21505,7 +21841,7 @@
       <c r="Z591" s="8"/>
     </row>
     <row r="592" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A592" s="9" t="s">
+      <c r="A592" s="3" t="s">
         <v>591</v>
       </c>
       <c r="B592" s="3"/>
@@ -21655,7 +21991,7 @@
       <c r="Z596" s="8"/>
     </row>
     <row r="597" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A597" s="3" t="s">
+      <c r="A597" s="9" t="s">
         <v>596</v>
       </c>
       <c r="B597" s="3"/>
@@ -21685,7 +22021,7 @@
       <c r="Z597" s="8"/>
     </row>
     <row r="598" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A598" s="9" t="s">
+      <c r="A598" s="3" t="s">
         <v>597</v>
       </c>
       <c r="B598" s="3"/>
@@ -21865,7 +22201,7 @@
       <c r="Z603" s="8"/>
     </row>
     <row r="604" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A604" s="3" t="s">
+      <c r="A604" s="9" t="s">
         <v>603</v>
       </c>
       <c r="B604" s="3"/>
@@ -21895,7 +22231,7 @@
       <c r="Z604" s="8"/>
     </row>
     <row r="605" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A605" s="9" t="s">
+      <c r="A605" s="3" t="s">
         <v>604</v>
       </c>
       <c r="B605" s="3"/>
@@ -21925,7 +22261,7 @@
       <c r="Z605" s="8"/>
     </row>
     <row r="606" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A606" s="3" t="s">
+      <c r="A606" s="9" t="s">
         <v>605</v>
       </c>
       <c r="B606" s="3"/>
@@ -21955,7 +22291,7 @@
       <c r="Z606" s="8"/>
     </row>
     <row r="607" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A607" s="9" t="s">
+      <c r="A607" s="3" t="s">
         <v>606</v>
       </c>
       <c r="B607" s="3"/>
@@ -22135,7 +22471,7 @@
       <c r="Z612" s="8"/>
     </row>
     <row r="613" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A613" s="3" t="s">
+      <c r="A613" s="9" t="s">
         <v>612</v>
       </c>
       <c r="B613" s="3"/>
@@ -22165,7 +22501,7 @@
       <c r="Z613" s="8"/>
     </row>
     <row r="614" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A614" s="9" t="s">
+      <c r="A614" s="3" t="s">
         <v>613</v>
       </c>
       <c r="B614" s="3"/>
@@ -22225,7 +22561,7 @@
       <c r="Z615" s="8"/>
     </row>
     <row r="616" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A616" s="3" t="s">
+      <c r="A616" s="9" t="s">
         <v>615</v>
       </c>
       <c r="B616" s="3"/>
@@ -22255,7 +22591,7 @@
       <c r="Z616" s="8"/>
     </row>
     <row r="617" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A617" s="9" t="s">
+      <c r="A617" s="3" t="s">
         <v>616</v>
       </c>
       <c r="B617" s="3"/>
@@ -22375,7 +22711,7 @@
       <c r="Z620" s="8"/>
     </row>
     <row r="621" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A621" s="3" t="s">
+      <c r="A621" s="9" t="s">
         <v>620</v>
       </c>
       <c r="B621" s="3"/>
@@ -22465,7 +22801,7 @@
       <c r="Z623" s="8"/>
     </row>
     <row r="624" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A624" s="9" t="s">
+      <c r="A624" s="3" t="s">
         <v>623</v>
       </c>
       <c r="B624" s="3"/>
@@ -22615,7 +22951,7 @@
       <c r="Z628" s="8"/>
     </row>
     <row r="629" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A629" s="3" t="s">
+      <c r="A629" s="9" t="s">
         <v>628</v>
       </c>
       <c r="B629" s="3"/>
@@ -22645,7 +22981,7 @@
       <c r="Z629" s="8"/>
     </row>
     <row r="630" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A630" s="9" t="s">
+      <c r="A630" s="3" t="s">
         <v>629</v>
       </c>
       <c r="B630" s="3"/>
@@ -22705,7 +23041,7 @@
       <c r="Z631" s="8"/>
     </row>
     <row r="632" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A632" s="3" t="s">
+      <c r="A632" s="9" t="s">
         <v>631</v>
       </c>
       <c r="B632" s="3"/>
@@ -22765,7 +23101,7 @@
       <c r="Z633" s="8"/>
     </row>
     <row r="634" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A634" s="9" t="s">
+      <c r="A634" s="3" t="s">
         <v>633</v>
       </c>
       <c r="B634" s="3"/>
@@ -23005,7 +23341,7 @@
       <c r="Z641" s="8"/>
     </row>
     <row r="642" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A642" s="3" t="s">
+      <c r="A642" s="9" t="s">
         <v>641</v>
       </c>
       <c r="B642" s="3"/>
@@ -23095,7 +23431,7 @@
       <c r="Z644" s="8"/>
     </row>
     <row r="645" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A645" s="9" t="s">
+      <c r="A645" s="3" t="s">
         <v>644</v>
       </c>
       <c r="B645" s="3"/>
@@ -23125,7 +23461,7 @@
       <c r="Z645" s="8"/>
     </row>
     <row r="646" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A646" s="3" t="s">
+      <c r="A646" s="9" t="s">
         <v>645</v>
       </c>
       <c r="B646" s="3"/>
@@ -23155,7 +23491,7 @@
       <c r="Z646" s="8"/>
     </row>
     <row r="647" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A647" s="9" t="s">
+      <c r="A647" s="3" t="s">
         <v>646</v>
       </c>
       <c r="B647" s="3"/>
@@ -23245,7 +23581,7 @@
       <c r="Z649" s="8"/>
     </row>
     <row r="650" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A650" s="3" t="s">
+      <c r="A650" s="9" t="s">
         <v>649</v>
       </c>
       <c r="B650" s="3"/>
@@ -23275,7 +23611,7 @@
       <c r="Z650" s="8"/>
     </row>
     <row r="651" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A651" s="9" t="s">
+      <c r="A651" s="3" t="s">
         <v>650</v>
       </c>
       <c r="B651" s="3"/>
@@ -23395,7 +23731,7 @@
       <c r="Z654" s="8"/>
     </row>
     <row r="655" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A655" s="3" t="s">
+      <c r="A655" s="9" t="s">
         <v>654</v>
       </c>
       <c r="B655" s="3"/>
@@ -23455,7 +23791,7 @@
       <c r="Z656" s="8"/>
     </row>
     <row r="657" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A657" s="9" t="s">
+      <c r="A657" s="3" t="s">
         <v>656</v>
       </c>
       <c r="B657" s="3"/>
@@ -23485,7 +23821,7 @@
       <c r="Z657" s="8"/>
     </row>
     <row r="658" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A658" s="3" t="s">
+      <c r="A658" s="9" t="s">
         <v>657</v>
       </c>
       <c r="B658" s="3"/>
@@ -23515,7 +23851,7 @@
       <c r="Z658" s="8"/>
     </row>
     <row r="659" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A659" s="9" t="s">
+      <c r="A659" s="3" t="s">
         <v>658</v>
       </c>
       <c r="B659" s="3"/>
@@ -23545,7 +23881,7 @@
       <c r="Z659" s="8"/>
     </row>
     <row r="660" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A660" s="3" t="s">
+      <c r="A660" s="5" t="s">
         <v>659</v>
       </c>
       <c r="B660" s="3"/>
@@ -23575,7 +23911,7 @@
       <c r="Z660" s="8"/>
     </row>
     <row r="661" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A661" s="5" t="s">
+      <c r="A661" s="3" t="s">
         <v>660</v>
       </c>
       <c r="B661" s="3"/>
@@ -23635,7 +23971,7 @@
       <c r="Z662" s="8"/>
     </row>
     <row r="663" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A663" s="3" t="s">
+      <c r="A663" s="9" t="s">
         <v>662</v>
       </c>
       <c r="B663" s="3"/>
@@ -23665,7 +24001,7 @@
       <c r="Z663" s="8"/>
     </row>
     <row r="664" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A664" s="9" t="s">
+      <c r="A664" s="3" t="s">
         <v>663</v>
       </c>
       <c r="B664" s="3"/>
@@ -23815,7 +24151,7 @@
       <c r="Z668" s="8"/>
     </row>
     <row r="669" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A669" s="3" t="s">
+      <c r="A669" s="9" t="s">
         <v>668</v>
       </c>
       <c r="B669" s="3"/>
@@ -23845,7 +24181,7 @@
       <c r="Z669" s="8"/>
     </row>
     <row r="670" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A670" s="9" t="s">
+      <c r="A670" s="3" t="s">
         <v>669</v>
       </c>
       <c r="B670" s="3"/>
@@ -23965,7 +24301,7 @@
       <c r="Z673" s="8"/>
     </row>
     <row r="674" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A674" s="3" t="s">
+      <c r="A674" s="7" t="s">
         <v>673</v>
       </c>
       <c r="B674" s="3"/>
@@ -23995,7 +24331,7 @@
       <c r="Z674" s="8"/>
     </row>
     <row r="675" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A675" s="7" t="s">
+      <c r="A675" s="3" t="s">
         <v>674</v>
       </c>
       <c r="B675" s="3"/>
@@ -24205,7 +24541,7 @@
       <c r="Z681" s="8"/>
     </row>
     <row r="682" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A682" s="3" t="s">
+      <c r="A682" s="5" t="s">
         <v>681</v>
       </c>
       <c r="B682" s="3"/>
@@ -24235,7 +24571,7 @@
       <c r="Z682" s="8"/>
     </row>
     <row r="683" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A683" s="5" t="s">
+      <c r="A683" s="3" t="s">
         <v>682</v>
       </c>
       <c r="B683" s="3"/>
@@ -24325,7 +24661,7 @@
       <c r="Z685" s="8"/>
     </row>
     <row r="686" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A686" s="3" t="s">
+      <c r="A686" s="10" t="s">
         <v>685</v>
       </c>
       <c r="B686" s="3"/>
@@ -24355,7 +24691,7 @@
       <c r="Z686" s="8"/>
     </row>
     <row r="687" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A687" s="10" t="s">
+      <c r="A687" s="9" t="s">
         <v>686</v>
       </c>
       <c r="B687" s="3"/>
@@ -24385,7 +24721,7 @@
       <c r="Z687" s="8"/>
     </row>
     <row r="688" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A688" s="9" t="s">
+      <c r="A688" s="3" t="s">
         <v>687</v>
       </c>
       <c r="B688" s="3"/>
@@ -24565,7 +24901,7 @@
       <c r="Z693" s="8"/>
     </row>
     <row r="694" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A694" s="3" t="s">
+      <c r="A694" s="9" t="s">
         <v>693</v>
       </c>
       <c r="B694" s="3"/>
@@ -24595,7 +24931,7 @@
       <c r="Z694" s="8"/>
     </row>
     <row r="695" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A695" s="9" t="s">
+      <c r="A695" s="3" t="s">
         <v>694</v>
       </c>
       <c r="B695" s="3"/>
@@ -24715,7 +25051,7 @@
       <c r="Z698" s="8"/>
     </row>
     <row r="699" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A699" s="3" t="s">
+      <c r="A699" s="9" t="s">
         <v>698</v>
       </c>
       <c r="B699" s="3"/>
@@ -24745,7 +25081,7 @@
       <c r="Z699" s="8"/>
     </row>
     <row r="700" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A700" s="9" t="s">
+      <c r="A700" s="3" t="s">
         <v>699</v>
       </c>
       <c r="B700" s="3"/>
@@ -25195,7 +25531,7 @@
       <c r="Z714" s="8"/>
     </row>
     <row r="715" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A715" s="3" t="s">
+      <c r="A715" s="5" t="s">
         <v>714</v>
       </c>
       <c r="B715" s="3"/>
@@ -25225,7 +25561,7 @@
       <c r="Z715" s="8"/>
     </row>
     <row r="716" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A716" s="5" t="s">
+      <c r="A716" s="3" t="s">
         <v>715</v>
       </c>
       <c r="B716" s="3"/>
@@ -25585,7 +25921,7 @@
       <c r="Z727" s="8"/>
     </row>
     <row r="728" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A728" s="3" t="s">
+      <c r="A728" s="5" t="s">
         <v>727</v>
       </c>
       <c r="B728" s="3"/>
@@ -25615,7 +25951,7 @@
       <c r="Z728" s="8"/>
     </row>
     <row r="729" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A729" s="5" t="s">
+      <c r="A729" s="3" t="s">
         <v>728</v>
       </c>
       <c r="B729" s="3"/>
@@ -26545,7 +26881,7 @@
       <c r="Z759" s="8"/>
     </row>
     <row r="760" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A760" s="3" t="s">
+      <c r="A760" s="7" t="s">
         <v>759</v>
       </c>
       <c r="B760" s="3"/>
@@ -26575,7 +26911,7 @@
       <c r="Z760" s="8"/>
     </row>
     <row r="761" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A761" s="7" t="s">
+      <c r="A761" s="3" t="s">
         <v>760</v>
       </c>
       <c r="B761" s="3"/>
@@ -27505,7 +27841,7 @@
       <c r="Z791" s="8"/>
     </row>
     <row r="792" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A792" s="3" t="s">
+      <c r="A792" s="7" t="s">
         <v>791</v>
       </c>
       <c r="B792" s="3"/>
@@ -27535,7 +27871,7 @@
       <c r="Z792" s="8"/>
     </row>
     <row r="793" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A793" s="7" t="s">
+      <c r="A793" s="3" t="s">
         <v>792</v>
       </c>
       <c r="B793" s="3"/>
@@ -27625,7 +27961,7 @@
       <c r="Z795" s="8"/>
     </row>
     <row r="796" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A796" s="3" t="s">
+      <c r="A796" s="6" t="s">
         <v>795</v>
       </c>
       <c r="B796" s="3"/>
@@ -27655,7 +27991,7 @@
       <c r="Z796" s="8"/>
     </row>
     <row r="797" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A797" s="6" t="s">
+      <c r="A797" s="3" t="s">
         <v>796</v>
       </c>
       <c r="B797" s="3"/>
@@ -28735,7 +29071,7 @@
       <c r="Z832" s="8"/>
     </row>
     <row r="833" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A833" s="3" t="s">
+      <c r="A833" s="5" t="s">
         <v>832</v>
       </c>
       <c r="B833" s="3"/>
@@ -28765,7 +29101,7 @@
       <c r="Z833" s="8"/>
     </row>
     <row r="834" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A834" s="5" t="s">
+      <c r="A834" s="3" t="s">
         <v>833</v>
       </c>
       <c r="B834" s="3"/>
@@ -29005,7 +29341,7 @@
       <c r="Z841" s="8"/>
     </row>
     <row r="842" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A842" s="3" t="s">
+      <c r="A842" s="9" t="s">
         <v>841</v>
       </c>
       <c r="B842" s="3"/>
@@ -29395,7 +29731,7 @@
       <c r="Z854" s="8"/>
     </row>
     <row r="855" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A855" s="9" t="s">
+      <c r="A855" s="3" t="s">
         <v>854</v>
       </c>
       <c r="B855" s="3"/>
@@ -29605,7 +29941,7 @@
       <c r="Z861" s="8"/>
     </row>
     <row r="862" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A862" s="3" t="s">
+      <c r="A862" s="8" t="s">
         <v>861</v>
       </c>
       <c r="B862" s="3"/>
@@ -29665,7 +30001,7 @@
       <c r="Z863" s="8"/>
     </row>
     <row r="864" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A864" s="8" t="s">
+      <c r="A864" s="11" t="s">
         <v>863</v>
       </c>
       <c r="B864" s="3"/>
@@ -29695,8 +30031,8 @@
       <c r="Z864" s="8"/>
     </row>
     <row r="865" ht="15.75" customHeight="1" spans="1:26">
-      <c r="A865" s="11" t="s">
-        <v>864</v>
+      <c r="A865" s="1" t="s">
+        <v>154</v>
       </c>
       <c r="B865" s="3"/>
       <c r="C865" s="3"/>
@@ -29726,7 +30062,7 @@
     </row>
     <row r="866" ht="15.75" customHeight="1" spans="1:26">
       <c r="A866" s="1" t="s">
-        <v>155</v>
+        <v>864</v>
       </c>
       <c r="B866" s="3"/>
       <c r="C866" s="3"/>
@@ -29756,7 +30092,7 @@
     </row>
     <row r="867" ht="15.75" customHeight="1" spans="1:26">
       <c r="A867" s="1" t="s">
-        <v>865</v>
+        <v>592</v>
       </c>
       <c r="B867" s="3"/>
       <c r="C867" s="3"/>
@@ -29786,7 +30122,7 @@
     </row>
     <row r="868" ht="15.75" customHeight="1" spans="1:26">
       <c r="A868" s="1" t="s">
-        <v>593</v>
+        <v>354</v>
       </c>
       <c r="B868" s="3"/>
       <c r="C868" s="3"/>
@@ -29816,7 +30152,7 @@
     </row>
     <row r="869" ht="15.75" customHeight="1" spans="1:26">
       <c r="A869" s="1" t="s">
-        <v>355</v>
+        <v>865</v>
       </c>
       <c r="B869" s="3"/>
       <c r="C869" s="3"/>
@@ -29968,8 +30304,8 @@
       <c r="A874" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="B874" s="3"/>
-      <c r="C874" s="3"/>
+      <c r="B874" s="4"/>
+      <c r="C874" s="4"/>
       <c r="D874" s="4"/>
       <c r="E874" s="4"/>
       <c r="F874" s="4"/>
@@ -30658,28 +30994,28 @@
       <c r="A897" s="1" t="s">
         <v>893</v>
       </c>
-      <c r="B897" s="4"/>
-      <c r="C897" s="4"/>
-      <c r="D897" s="4"/>
-      <c r="E897" s="4"/>
-      <c r="F897" s="4"/>
-      <c r="G897" s="4"/>
-      <c r="H897" s="4"/>
-      <c r="I897" s="4"/>
-      <c r="J897" s="4"/>
-      <c r="K897" s="4"/>
-      <c r="L897" s="4"/>
-      <c r="M897" s="4"/>
-      <c r="N897" s="4"/>
-      <c r="O897" s="4"/>
-      <c r="P897" s="4"/>
-      <c r="Q897" s="4"/>
-      <c r="R897" s="4"/>
-      <c r="S897" s="4"/>
-      <c r="T897" s="4"/>
-      <c r="U897" s="4"/>
-      <c r="V897" s="4"/>
-      <c r="W897" s="4"/>
+      <c r="B897" s="8"/>
+      <c r="C897" s="8"/>
+      <c r="D897" s="8"/>
+      <c r="E897" s="8"/>
+      <c r="F897" s="8"/>
+      <c r="G897" s="8"/>
+      <c r="H897" s="8"/>
+      <c r="I897" s="8"/>
+      <c r="J897" s="8"/>
+      <c r="K897" s="8"/>
+      <c r="L897" s="8"/>
+      <c r="M897" s="8"/>
+      <c r="N897" s="8"/>
+      <c r="O897" s="8"/>
+      <c r="P897" s="8"/>
+      <c r="Q897" s="8"/>
+      <c r="R897" s="8"/>
+      <c r="S897" s="8"/>
+      <c r="T897" s="8"/>
+      <c r="U897" s="8"/>
+      <c r="V897" s="8"/>
+      <c r="W897" s="8"/>
       <c r="X897" s="8"/>
       <c r="Y897" s="8"/>
       <c r="Z897" s="8"/>
@@ -30924,7 +31260,10 @@
       <c r="Y905" s="8"/>
       <c r="Z905" s="8"/>
     </row>
-    <row r="906" ht="15.75" customHeight="1" spans="2:26">
+    <row r="906" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A906" s="1" t="s">
+        <v>902</v>
+      </c>
       <c r="B906" s="8"/>
       <c r="C906" s="8"/>
       <c r="D906" s="8"/>
@@ -30951,7 +31290,10 @@
       <c r="Y906" s="8"/>
       <c r="Z906" s="8"/>
     </row>
-    <row r="907" ht="15.75" customHeight="1" spans="2:26">
+    <row r="907" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A907" s="1" t="s">
+        <v>903</v>
+      </c>
       <c r="B907" s="8"/>
       <c r="C907" s="8"/>
       <c r="D907" s="8"/>
@@ -30978,7 +31320,10 @@
       <c r="Y907" s="8"/>
       <c r="Z907" s="8"/>
     </row>
-    <row r="908" ht="15.75" customHeight="1" spans="2:26">
+    <row r="908" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A908" s="1" t="s">
+        <v>904</v>
+      </c>
       <c r="B908" s="8"/>
       <c r="C908" s="8"/>
       <c r="D908" s="8"/>
@@ -31005,7 +31350,10 @@
       <c r="Y908" s="8"/>
       <c r="Z908" s="8"/>
     </row>
-    <row r="909" ht="15.75" customHeight="1" spans="2:26">
+    <row r="909" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A909" s="1" t="s">
+        <v>905</v>
+      </c>
       <c r="B909" s="8"/>
       <c r="C909" s="8"/>
       <c r="D909" s="8"/>
@@ -31032,7 +31380,10 @@
       <c r="Y909" s="8"/>
       <c r="Z909" s="8"/>
     </row>
-    <row r="910" ht="15.75" customHeight="1" spans="2:26">
+    <row r="910" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A910" s="1" t="s">
+        <v>906</v>
+      </c>
       <c r="B910" s="8"/>
       <c r="C910" s="8"/>
       <c r="D910" s="8"/>
@@ -31059,7 +31410,10 @@
       <c r="Y910" s="8"/>
       <c r="Z910" s="8"/>
     </row>
-    <row r="911" ht="15.75" customHeight="1" spans="2:26">
+    <row r="911" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A911" s="1" t="s">
+        <v>907</v>
+      </c>
       <c r="B911" s="8"/>
       <c r="C911" s="8"/>
       <c r="D911" s="8"/>
@@ -31086,7 +31440,10 @@
       <c r="Y911" s="8"/>
       <c r="Z911" s="8"/>
     </row>
-    <row r="912" ht="15.75" customHeight="1" spans="2:26">
+    <row r="912" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A912" s="1" t="s">
+        <v>908</v>
+      </c>
       <c r="B912" s="8"/>
       <c r="C912" s="8"/>
       <c r="D912" s="8"/>
@@ -31113,7 +31470,10 @@
       <c r="Y912" s="8"/>
       <c r="Z912" s="8"/>
     </row>
-    <row r="913" ht="15.75" customHeight="1" spans="2:26">
+    <row r="913" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A913" s="1" t="s">
+        <v>909</v>
+      </c>
       <c r="B913" s="8"/>
       <c r="C913" s="8"/>
       <c r="D913" s="8"/>
@@ -31140,7 +31500,10 @@
       <c r="Y913" s="8"/>
       <c r="Z913" s="8"/>
     </row>
-    <row r="914" ht="15.75" customHeight="1" spans="2:26">
+    <row r="914" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A914" s="1" t="s">
+        <v>910</v>
+      </c>
       <c r="B914" s="8"/>
       <c r="C914" s="8"/>
       <c r="D914" s="8"/>
@@ -31167,7 +31530,10 @@
       <c r="Y914" s="8"/>
       <c r="Z914" s="8"/>
     </row>
-    <row r="915" ht="15.75" customHeight="1" spans="2:26">
+    <row r="915" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A915" s="1" t="s">
+        <v>911</v>
+      </c>
       <c r="B915" s="8"/>
       <c r="C915" s="8"/>
       <c r="D915" s="8"/>
@@ -31194,7 +31560,10 @@
       <c r="Y915" s="8"/>
       <c r="Z915" s="8"/>
     </row>
-    <row r="916" ht="15.75" customHeight="1" spans="2:26">
+    <row r="916" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A916" s="1" t="s">
+        <v>912</v>
+      </c>
       <c r="B916" s="8"/>
       <c r="C916" s="8"/>
       <c r="D916" s="8"/>
@@ -31221,7 +31590,10 @@
       <c r="Y916" s="8"/>
       <c r="Z916" s="8"/>
     </row>
-    <row r="917" ht="15.75" customHeight="1" spans="2:26">
+    <row r="917" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A917" s="1" t="s">
+        <v>913</v>
+      </c>
       <c r="B917" s="8"/>
       <c r="C917" s="8"/>
       <c r="D917" s="8"/>
@@ -31248,7 +31620,10 @@
       <c r="Y917" s="8"/>
       <c r="Z917" s="8"/>
     </row>
-    <row r="918" ht="15.75" customHeight="1" spans="2:26">
+    <row r="918" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A918" s="1" t="s">
+        <v>914</v>
+      </c>
       <c r="B918" s="8"/>
       <c r="C918" s="8"/>
       <c r="D918" s="8"/>
@@ -31275,7 +31650,10 @@
       <c r="Y918" s="8"/>
       <c r="Z918" s="8"/>
     </row>
-    <row r="919" ht="15.75" customHeight="1" spans="2:26">
+    <row r="919" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A919" s="1" t="s">
+        <v>915</v>
+      </c>
       <c r="B919" s="8"/>
       <c r="C919" s="8"/>
       <c r="D919" s="8"/>
@@ -31302,7 +31680,10 @@
       <c r="Y919" s="8"/>
       <c r="Z919" s="8"/>
     </row>
-    <row r="920" ht="15.75" customHeight="1" spans="2:26">
+    <row r="920" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A920" s="1" t="s">
+        <v>916</v>
+      </c>
       <c r="B920" s="8"/>
       <c r="C920" s="8"/>
       <c r="D920" s="8"/>
@@ -31329,7 +31710,10 @@
       <c r="Y920" s="8"/>
       <c r="Z920" s="8"/>
     </row>
-    <row r="921" ht="15.75" customHeight="1" spans="2:26">
+    <row r="921" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A921" s="1" t="s">
+        <v>917</v>
+      </c>
       <c r="B921" s="8"/>
       <c r="C921" s="8"/>
       <c r="D921" s="8"/>
@@ -31356,7 +31740,10 @@
       <c r="Y921" s="8"/>
       <c r="Z921" s="8"/>
     </row>
-    <row r="922" ht="15.75" customHeight="1" spans="2:26">
+    <row r="922" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A922" s="1" t="s">
+        <v>918</v>
+      </c>
       <c r="B922" s="8"/>
       <c r="C922" s="8"/>
       <c r="D922" s="8"/>
@@ -31383,7 +31770,10 @@
       <c r="Y922" s="8"/>
       <c r="Z922" s="8"/>
     </row>
-    <row r="923" ht="15.75" customHeight="1" spans="2:26">
+    <row r="923" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A923" s="1" t="s">
+        <v>919</v>
+      </c>
       <c r="B923" s="8"/>
       <c r="C923" s="8"/>
       <c r="D923" s="8"/>
@@ -31410,7 +31800,10 @@
       <c r="Y923" s="8"/>
       <c r="Z923" s="8"/>
     </row>
-    <row r="924" ht="15.75" customHeight="1" spans="2:26">
+    <row r="924" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A924" s="1" t="s">
+        <v>920</v>
+      </c>
       <c r="B924" s="8"/>
       <c r="C924" s="8"/>
       <c r="D924" s="8"/>
@@ -31437,7 +31830,10 @@
       <c r="Y924" s="8"/>
       <c r="Z924" s="8"/>
     </row>
-    <row r="925" ht="15.75" customHeight="1" spans="2:26">
+    <row r="925" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A925" s="1" t="s">
+        <v>921</v>
+      </c>
       <c r="B925" s="8"/>
       <c r="C925" s="8"/>
       <c r="D925" s="8"/>
@@ -31464,7 +31860,10 @@
       <c r="Y925" s="8"/>
       <c r="Z925" s="8"/>
     </row>
-    <row r="926" ht="15.75" customHeight="1" spans="2:26">
+    <row r="926" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A926" s="1" t="s">
+        <v>922</v>
+      </c>
       <c r="B926" s="8"/>
       <c r="C926" s="8"/>
       <c r="D926" s="8"/>
@@ -31491,7 +31890,10 @@
       <c r="Y926" s="8"/>
       <c r="Z926" s="8"/>
     </row>
-    <row r="927" ht="15.75" customHeight="1" spans="2:26">
+    <row r="927" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A927" s="1" t="s">
+        <v>923</v>
+      </c>
       <c r="B927" s="8"/>
       <c r="C927" s="8"/>
       <c r="D927" s="8"/>
@@ -31518,7 +31920,10 @@
       <c r="Y927" s="8"/>
       <c r="Z927" s="8"/>
     </row>
-    <row r="928" ht="15.75" customHeight="1" spans="2:26">
+    <row r="928" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A928" s="1" t="s">
+        <v>924</v>
+      </c>
       <c r="B928" s="8"/>
       <c r="C928" s="8"/>
       <c r="D928" s="8"/>
@@ -31545,7 +31950,10 @@
       <c r="Y928" s="8"/>
       <c r="Z928" s="8"/>
     </row>
-    <row r="929" ht="15.75" customHeight="1" spans="2:26">
+    <row r="929" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A929" s="1" t="s">
+        <v>925</v>
+      </c>
       <c r="B929" s="8"/>
       <c r="C929" s="8"/>
       <c r="D929" s="8"/>
@@ -31572,7 +31980,10 @@
       <c r="Y929" s="8"/>
       <c r="Z929" s="8"/>
     </row>
-    <row r="930" ht="15.75" customHeight="1" spans="2:26">
+    <row r="930" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A930" s="1" t="s">
+        <v>926</v>
+      </c>
       <c r="B930" s="8"/>
       <c r="C930" s="8"/>
       <c r="D930" s="8"/>
@@ -31599,7 +32010,10 @@
       <c r="Y930" s="8"/>
       <c r="Z930" s="8"/>
     </row>
-    <row r="931" ht="15.75" customHeight="1" spans="2:26">
+    <row r="931" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A931" s="1" t="s">
+        <v>927</v>
+      </c>
       <c r="B931" s="8"/>
       <c r="C931" s="8"/>
       <c r="D931" s="8"/>
@@ -31626,7 +32040,10 @@
       <c r="Y931" s="8"/>
       <c r="Z931" s="8"/>
     </row>
-    <row r="932" ht="15.75" customHeight="1" spans="2:26">
+    <row r="932" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A932" s="1" t="s">
+        <v>928</v>
+      </c>
       <c r="B932" s="8"/>
       <c r="C932" s="8"/>
       <c r="D932" s="8"/>
@@ -31653,7 +32070,10 @@
       <c r="Y932" s="8"/>
       <c r="Z932" s="8"/>
     </row>
-    <row r="933" ht="15.75" customHeight="1" spans="2:26">
+    <row r="933" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A933" s="1" t="s">
+        <v>929</v>
+      </c>
       <c r="B933" s="8"/>
       <c r="C933" s="8"/>
       <c r="D933" s="8"/>
@@ -31680,7 +32100,10 @@
       <c r="Y933" s="8"/>
       <c r="Z933" s="8"/>
     </row>
-    <row r="934" ht="15.75" customHeight="1" spans="2:26">
+    <row r="934" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A934" s="1" t="s">
+        <v>930</v>
+      </c>
       <c r="B934" s="8"/>
       <c r="C934" s="8"/>
       <c r="D934" s="8"/>
@@ -31707,7 +32130,10 @@
       <c r="Y934" s="8"/>
       <c r="Z934" s="8"/>
     </row>
-    <row r="935" ht="15.75" customHeight="1" spans="2:26">
+    <row r="935" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A935" s="1" t="s">
+        <v>931</v>
+      </c>
       <c r="B935" s="8"/>
       <c r="C935" s="8"/>
       <c r="D935" s="8"/>
@@ -31734,7 +32160,10 @@
       <c r="Y935" s="8"/>
       <c r="Z935" s="8"/>
     </row>
-    <row r="936" ht="15.75" customHeight="1" spans="2:26">
+    <row r="936" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A936" s="1" t="s">
+        <v>932</v>
+      </c>
       <c r="B936" s="8"/>
       <c r="C936" s="8"/>
       <c r="D936" s="8"/>
@@ -31761,7 +32190,10 @@
       <c r="Y936" s="8"/>
       <c r="Z936" s="8"/>
     </row>
-    <row r="937" ht="15.75" customHeight="1" spans="2:26">
+    <row r="937" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A937" s="1" t="s">
+        <v>933</v>
+      </c>
       <c r="B937" s="8"/>
       <c r="C937" s="8"/>
       <c r="D937" s="8"/>
@@ -31788,7 +32220,10 @@
       <c r="Y937" s="8"/>
       <c r="Z937" s="8"/>
     </row>
-    <row r="938" ht="15.75" customHeight="1" spans="2:26">
+    <row r="938" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A938" s="1" t="s">
+        <v>934</v>
+      </c>
       <c r="B938" s="8"/>
       <c r="C938" s="8"/>
       <c r="D938" s="8"/>
@@ -31815,7 +32250,10 @@
       <c r="Y938" s="8"/>
       <c r="Z938" s="8"/>
     </row>
-    <row r="939" ht="15.75" customHeight="1" spans="2:26">
+    <row r="939" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A939" s="1" t="s">
+        <v>935</v>
+      </c>
       <c r="B939" s="8"/>
       <c r="C939" s="8"/>
       <c r="D939" s="8"/>
@@ -31842,7 +32280,10 @@
       <c r="Y939" s="8"/>
       <c r="Z939" s="8"/>
     </row>
-    <row r="940" ht="15.75" customHeight="1" spans="2:26">
+    <row r="940" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A940" s="1" t="s">
+        <v>936</v>
+      </c>
       <c r="B940" s="8"/>
       <c r="C940" s="8"/>
       <c r="D940" s="8"/>
@@ -31869,7 +32310,10 @@
       <c r="Y940" s="8"/>
       <c r="Z940" s="8"/>
     </row>
-    <row r="941" ht="15.75" customHeight="1" spans="2:26">
+    <row r="941" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A941" s="1" t="s">
+        <v>937</v>
+      </c>
       <c r="B941" s="8"/>
       <c r="C941" s="8"/>
       <c r="D941" s="8"/>
@@ -31896,7 +32340,10 @@
       <c r="Y941" s="8"/>
       <c r="Z941" s="8"/>
     </row>
-    <row r="942" ht="15.75" customHeight="1" spans="2:26">
+    <row r="942" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A942" s="1" t="s">
+        <v>938</v>
+      </c>
       <c r="B942" s="8"/>
       <c r="C942" s="8"/>
       <c r="D942" s="8"/>
@@ -31923,7 +32370,10 @@
       <c r="Y942" s="8"/>
       <c r="Z942" s="8"/>
     </row>
-    <row r="943" ht="15.75" customHeight="1" spans="2:26">
+    <row r="943" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A943" s="1" t="s">
+        <v>939</v>
+      </c>
       <c r="B943" s="8"/>
       <c r="C943" s="8"/>
       <c r="D943" s="8"/>
@@ -31950,7 +32400,10 @@
       <c r="Y943" s="8"/>
       <c r="Z943" s="8"/>
     </row>
-    <row r="944" ht="15.75" customHeight="1" spans="2:26">
+    <row r="944" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A944" s="1" t="s">
+        <v>940</v>
+      </c>
       <c r="B944" s="8"/>
       <c r="C944" s="8"/>
       <c r="D944" s="8"/>
@@ -31977,7 +32430,10 @@
       <c r="Y944" s="8"/>
       <c r="Z944" s="8"/>
     </row>
-    <row r="945" ht="15.75" customHeight="1" spans="2:26">
+    <row r="945" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A945" s="1" t="s">
+        <v>941</v>
+      </c>
       <c r="B945" s="8"/>
       <c r="C945" s="8"/>
       <c r="D945" s="8"/>
@@ -32004,7 +32460,10 @@
       <c r="Y945" s="8"/>
       <c r="Z945" s="8"/>
     </row>
-    <row r="946" ht="15.75" customHeight="1" spans="2:26">
+    <row r="946" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A946" s="1" t="s">
+        <v>942</v>
+      </c>
       <c r="B946" s="8"/>
       <c r="C946" s="8"/>
       <c r="D946" s="8"/>
@@ -32031,7 +32490,10 @@
       <c r="Y946" s="8"/>
       <c r="Z946" s="8"/>
     </row>
-    <row r="947" ht="15.75" customHeight="1" spans="2:26">
+    <row r="947" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A947" s="1" t="s">
+        <v>943</v>
+      </c>
       <c r="B947" s="8"/>
       <c r="C947" s="8"/>
       <c r="D947" s="8"/>
@@ -32058,7 +32520,10 @@
       <c r="Y947" s="8"/>
       <c r="Z947" s="8"/>
     </row>
-    <row r="948" ht="15.75" customHeight="1" spans="2:26">
+    <row r="948" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A948" s="1" t="s">
+        <v>944</v>
+      </c>
       <c r="B948" s="8"/>
       <c r="C948" s="8"/>
       <c r="D948" s="8"/>
@@ -32085,7 +32550,10 @@
       <c r="Y948" s="8"/>
       <c r="Z948" s="8"/>
     </row>
-    <row r="949" ht="15.75" customHeight="1" spans="2:26">
+    <row r="949" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A949" s="1" t="s">
+        <v>945</v>
+      </c>
       <c r="B949" s="8"/>
       <c r="C949" s="8"/>
       <c r="D949" s="8"/>
@@ -32112,7 +32580,10 @@
       <c r="Y949" s="8"/>
       <c r="Z949" s="8"/>
     </row>
-    <row r="950" ht="15.75" customHeight="1" spans="2:26">
+    <row r="950" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A950" s="1" t="s">
+        <v>946</v>
+      </c>
       <c r="B950" s="8"/>
       <c r="C950" s="8"/>
       <c r="D950" s="8"/>
@@ -32139,7 +32610,10 @@
       <c r="Y950" s="8"/>
       <c r="Z950" s="8"/>
     </row>
-    <row r="951" ht="15.75" customHeight="1" spans="2:26">
+    <row r="951" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A951" s="1" t="s">
+        <v>947</v>
+      </c>
       <c r="B951" s="8"/>
       <c r="C951" s="8"/>
       <c r="D951" s="8"/>
@@ -32166,7 +32640,10 @@
       <c r="Y951" s="8"/>
       <c r="Z951" s="8"/>
     </row>
-    <row r="952" ht="15.75" customHeight="1" spans="2:26">
+    <row r="952" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A952" s="1" t="s">
+        <v>948</v>
+      </c>
       <c r="B952" s="8"/>
       <c r="C952" s="8"/>
       <c r="D952" s="8"/>
@@ -32193,7 +32670,10 @@
       <c r="Y952" s="8"/>
       <c r="Z952" s="8"/>
     </row>
-    <row r="953" ht="15.75" customHeight="1" spans="2:26">
+    <row r="953" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A953" s="1" t="s">
+        <v>949</v>
+      </c>
       <c r="B953" s="8"/>
       <c r="C953" s="8"/>
       <c r="D953" s="8"/>
@@ -32220,7 +32700,10 @@
       <c r="Y953" s="8"/>
       <c r="Z953" s="8"/>
     </row>
-    <row r="954" ht="15.75" customHeight="1" spans="2:26">
+    <row r="954" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A954" s="1" t="s">
+        <v>950</v>
+      </c>
       <c r="B954" s="8"/>
       <c r="C954" s="8"/>
       <c r="D954" s="8"/>
@@ -32247,7 +32730,10 @@
       <c r="Y954" s="8"/>
       <c r="Z954" s="8"/>
     </row>
-    <row r="955" ht="15.75" customHeight="1" spans="2:26">
+    <row r="955" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A955" s="1" t="s">
+        <v>951</v>
+      </c>
       <c r="B955" s="8"/>
       <c r="C955" s="8"/>
       <c r="D955" s="8"/>
@@ -32274,7 +32760,10 @@
       <c r="Y955" s="8"/>
       <c r="Z955" s="8"/>
     </row>
-    <row r="956" ht="15.75" customHeight="1" spans="2:26">
+    <row r="956" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A956" s="1" t="s">
+        <v>952</v>
+      </c>
       <c r="B956" s="8"/>
       <c r="C956" s="8"/>
       <c r="D956" s="8"/>
@@ -32301,7 +32790,10 @@
       <c r="Y956" s="8"/>
       <c r="Z956" s="8"/>
     </row>
-    <row r="957" ht="15.75" customHeight="1" spans="2:26">
+    <row r="957" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A957" s="1" t="s">
+        <v>953</v>
+      </c>
       <c r="B957" s="8"/>
       <c r="C957" s="8"/>
       <c r="D957" s="8"/>
@@ -32328,7 +32820,10 @@
       <c r="Y957" s="8"/>
       <c r="Z957" s="8"/>
     </row>
-    <row r="958" ht="15.75" customHeight="1" spans="2:26">
+    <row r="958" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A958" s="1" t="s">
+        <v>954</v>
+      </c>
       <c r="B958" s="8"/>
       <c r="C958" s="8"/>
       <c r="D958" s="8"/>
@@ -32355,7 +32850,10 @@
       <c r="Y958" s="8"/>
       <c r="Z958" s="8"/>
     </row>
-    <row r="959" ht="15.75" customHeight="1" spans="2:26">
+    <row r="959" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A959" s="1" t="s">
+        <v>955</v>
+      </c>
       <c r="B959" s="8"/>
       <c r="C959" s="8"/>
       <c r="D959" s="8"/>
@@ -32382,7 +32880,10 @@
       <c r="Y959" s="8"/>
       <c r="Z959" s="8"/>
     </row>
-    <row r="960" ht="15.75" customHeight="1" spans="2:26">
+    <row r="960" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A960" s="1" t="s">
+        <v>956</v>
+      </c>
       <c r="B960" s="8"/>
       <c r="C960" s="8"/>
       <c r="D960" s="8"/>
@@ -32409,7 +32910,10 @@
       <c r="Y960" s="8"/>
       <c r="Z960" s="8"/>
     </row>
-    <row r="961" ht="15.75" customHeight="1" spans="2:26">
+    <row r="961" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A961" s="12" t="s">
+        <v>957</v>
+      </c>
       <c r="B961" s="8"/>
       <c r="C961" s="8"/>
       <c r="D961" s="8"/>
@@ -32436,7 +32940,10 @@
       <c r="Y961" s="8"/>
       <c r="Z961" s="8"/>
     </row>
-    <row r="962" ht="15.75" customHeight="1" spans="2:26">
+    <row r="962" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A962" s="1" t="s">
+        <v>958</v>
+      </c>
       <c r="B962" s="8"/>
       <c r="C962" s="8"/>
       <c r="D962" s="8"/>
@@ -32463,7 +32970,10 @@
       <c r="Y962" s="8"/>
       <c r="Z962" s="8"/>
     </row>
-    <row r="963" ht="15.75" customHeight="1" spans="2:26">
+    <row r="963" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A963" s="1" t="s">
+        <v>959</v>
+      </c>
       <c r="B963" s="8"/>
       <c r="C963" s="8"/>
       <c r="D963" s="8"/>
@@ -32490,7 +33000,10 @@
       <c r="Y963" s="8"/>
       <c r="Z963" s="8"/>
     </row>
-    <row r="964" ht="15.75" customHeight="1" spans="2:26">
+    <row r="964" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A964" s="12" t="s">
+        <v>960</v>
+      </c>
       <c r="B964" s="8"/>
       <c r="C964" s="8"/>
       <c r="D964" s="8"/>
@@ -32517,7 +33030,10 @@
       <c r="Y964" s="8"/>
       <c r="Z964" s="8"/>
     </row>
-    <row r="965" ht="15.75" customHeight="1" spans="2:26">
+    <row r="965" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A965" s="1" t="s">
+        <v>958</v>
+      </c>
       <c r="B965" s="8"/>
       <c r="C965" s="8"/>
       <c r="D965" s="8"/>
@@ -32544,7 +33060,10 @@
       <c r="Y965" s="8"/>
       <c r="Z965" s="8"/>
     </row>
-    <row r="966" ht="15.75" customHeight="1" spans="2:26">
+    <row r="966" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A966" s="1" t="s">
+        <v>961</v>
+      </c>
       <c r="B966" s="8"/>
       <c r="C966" s="8"/>
       <c r="D966" s="8"/>
@@ -32571,7 +33090,10 @@
       <c r="Y966" s="8"/>
       <c r="Z966" s="8"/>
     </row>
-    <row r="967" ht="15.75" customHeight="1" spans="2:26">
+    <row r="967" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A967" s="1" t="s">
+        <v>962</v>
+      </c>
       <c r="B967" s="8"/>
       <c r="C967" s="8"/>
       <c r="D967" s="8"/>
@@ -32598,7 +33120,10 @@
       <c r="Y967" s="8"/>
       <c r="Z967" s="8"/>
     </row>
-    <row r="968" ht="15.75" customHeight="1" spans="2:26">
+    <row r="968" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A968" s="1" t="s">
+        <v>963</v>
+      </c>
       <c r="B968" s="8"/>
       <c r="C968" s="8"/>
       <c r="D968" s="8"/>
@@ -32625,7 +33150,10 @@
       <c r="Y968" s="8"/>
       <c r="Z968" s="8"/>
     </row>
-    <row r="969" ht="15.75" customHeight="1" spans="2:26">
+    <row r="969" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A969" s="1" t="s">
+        <v>964</v>
+      </c>
       <c r="B969" s="8"/>
       <c r="C969" s="8"/>
       <c r="D969" s="8"/>
@@ -32652,7 +33180,10 @@
       <c r="Y969" s="8"/>
       <c r="Z969" s="8"/>
     </row>
-    <row r="970" ht="15.75" customHeight="1" spans="2:26">
+    <row r="970" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A970" s="1" t="s">
+        <v>965</v>
+      </c>
       <c r="B970" s="8"/>
       <c r="C970" s="8"/>
       <c r="D970" s="8"/>
@@ -32679,7 +33210,10 @@
       <c r="Y970" s="8"/>
       <c r="Z970" s="8"/>
     </row>
-    <row r="971" ht="15.75" customHeight="1" spans="2:26">
+    <row r="971" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A971" s="1" t="s">
+        <v>966</v>
+      </c>
       <c r="B971" s="8"/>
       <c r="C971" s="8"/>
       <c r="D971" s="8"/>
@@ -32706,7 +33240,10 @@
       <c r="Y971" s="8"/>
       <c r="Z971" s="8"/>
     </row>
-    <row r="972" ht="15.75" customHeight="1" spans="2:26">
+    <row r="972" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A972" s="1" t="s">
+        <v>967</v>
+      </c>
       <c r="B972" s="8"/>
       <c r="C972" s="8"/>
       <c r="D972" s="8"/>
@@ -32733,7 +33270,10 @@
       <c r="Y972" s="8"/>
       <c r="Z972" s="8"/>
     </row>
-    <row r="973" ht="15.75" customHeight="1" spans="2:26">
+    <row r="973" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A973" s="1" t="s">
+        <v>968</v>
+      </c>
       <c r="B973" s="8"/>
       <c r="C973" s="8"/>
       <c r="D973" s="8"/>
@@ -32760,7 +33300,10 @@
       <c r="Y973" s="8"/>
       <c r="Z973" s="8"/>
     </row>
-    <row r="974" ht="15.75" customHeight="1" spans="2:26">
+    <row r="974" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A974" s="1" t="s">
+        <v>969</v>
+      </c>
       <c r="B974" s="8"/>
       <c r="C974" s="8"/>
       <c r="D974" s="8"/>
@@ -32787,7 +33330,10 @@
       <c r="Y974" s="8"/>
       <c r="Z974" s="8"/>
     </row>
-    <row r="975" ht="15.75" customHeight="1" spans="2:26">
+    <row r="975" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A975" s="1" t="s">
+        <v>970</v>
+      </c>
       <c r="B975" s="8"/>
       <c r="C975" s="8"/>
       <c r="D975" s="8"/>
@@ -32814,7 +33360,10 @@
       <c r="Y975" s="8"/>
       <c r="Z975" s="8"/>
     </row>
-    <row r="976" ht="15.75" customHeight="1" spans="2:26">
+    <row r="976" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A976" s="1" t="s">
+        <v>971</v>
+      </c>
       <c r="B976" s="8"/>
       <c r="C976" s="8"/>
       <c r="D976" s="8"/>
@@ -32841,7 +33390,10 @@
       <c r="Y976" s="8"/>
       <c r="Z976" s="8"/>
     </row>
-    <row r="977" ht="15.75" customHeight="1" spans="2:26">
+    <row r="977" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A977" s="1" t="s">
+        <v>972</v>
+      </c>
       <c r="B977" s="8"/>
       <c r="C977" s="8"/>
       <c r="D977" s="8"/>
@@ -32868,7 +33420,10 @@
       <c r="Y977" s="8"/>
       <c r="Z977" s="8"/>
     </row>
-    <row r="978" ht="15.75" customHeight="1" spans="2:26">
+    <row r="978" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A978" s="1" t="s">
+        <v>973</v>
+      </c>
       <c r="B978" s="8"/>
       <c r="C978" s="8"/>
       <c r="D978" s="8"/>
@@ -32895,7 +33450,10 @@
       <c r="Y978" s="8"/>
       <c r="Z978" s="8"/>
     </row>
-    <row r="979" ht="15.75" customHeight="1" spans="2:26">
+    <row r="979" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A979" s="1" t="s">
+        <v>974</v>
+      </c>
       <c r="B979" s="8"/>
       <c r="C979" s="8"/>
       <c r="D979" s="8"/>
@@ -32922,7 +33480,10 @@
       <c r="Y979" s="8"/>
       <c r="Z979" s="8"/>
     </row>
-    <row r="980" ht="15.75" customHeight="1" spans="2:26">
+    <row r="980" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A980" s="1" t="s">
+        <v>975</v>
+      </c>
       <c r="B980" s="8"/>
       <c r="C980" s="8"/>
       <c r="D980" s="8"/>
@@ -32949,7 +33510,10 @@
       <c r="Y980" s="8"/>
       <c r="Z980" s="8"/>
     </row>
-    <row r="981" ht="15.75" customHeight="1" spans="2:26">
+    <row r="981" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A981" s="1" t="s">
+        <v>976</v>
+      </c>
       <c r="B981" s="8"/>
       <c r="C981" s="8"/>
       <c r="D981" s="8"/>
@@ -32976,7 +33540,10 @@
       <c r="Y981" s="8"/>
       <c r="Z981" s="8"/>
     </row>
-    <row r="982" ht="15.75" customHeight="1" spans="2:26">
+    <row r="982" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A982" s="1" t="s">
+        <v>977</v>
+      </c>
       <c r="B982" s="8"/>
       <c r="C982" s="8"/>
       <c r="D982" s="8"/>
@@ -33003,7 +33570,10 @@
       <c r="Y982" s="8"/>
       <c r="Z982" s="8"/>
     </row>
-    <row r="983" ht="15.75" customHeight="1" spans="2:26">
+    <row r="983" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A983" s="1" t="s">
+        <v>978</v>
+      </c>
       <c r="B983" s="8"/>
       <c r="C983" s="8"/>
       <c r="D983" s="8"/>
@@ -33030,7 +33600,10 @@
       <c r="Y983" s="8"/>
       <c r="Z983" s="8"/>
     </row>
-    <row r="984" ht="15.75" customHeight="1" spans="2:26">
+    <row r="984" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A984" s="1" t="s">
+        <v>979</v>
+      </c>
       <c r="B984" s="8"/>
       <c r="C984" s="8"/>
       <c r="D984" s="8"/>
@@ -33057,7 +33630,10 @@
       <c r="Y984" s="8"/>
       <c r="Z984" s="8"/>
     </row>
-    <row r="985" ht="15.75" customHeight="1" spans="2:26">
+    <row r="985" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A985" s="1" t="s">
+        <v>980</v>
+      </c>
       <c r="B985" s="8"/>
       <c r="C985" s="8"/>
       <c r="D985" s="8"/>
@@ -33084,7 +33660,10 @@
       <c r="Y985" s="8"/>
       <c r="Z985" s="8"/>
     </row>
-    <row r="986" ht="15.75" customHeight="1" spans="2:26">
+    <row r="986" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A986" s="1" t="s">
+        <v>278</v>
+      </c>
       <c r="B986" s="8"/>
       <c r="C986" s="8"/>
       <c r="D986" s="8"/>
@@ -33111,7 +33690,10 @@
       <c r="Y986" s="8"/>
       <c r="Z986" s="8"/>
     </row>
-    <row r="987" ht="15.75" customHeight="1" spans="2:26">
+    <row r="987" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A987" s="1" t="s">
+        <v>981</v>
+      </c>
       <c r="B987" s="8"/>
       <c r="C987" s="8"/>
       <c r="D987" s="8"/>
@@ -33138,7 +33720,10 @@
       <c r="Y987" s="8"/>
       <c r="Z987" s="8"/>
     </row>
-    <row r="988" ht="15.75" customHeight="1" spans="2:26">
+    <row r="988" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A988" s="1" t="s">
+        <v>982</v>
+      </c>
       <c r="B988" s="8"/>
       <c r="C988" s="8"/>
       <c r="D988" s="8"/>
@@ -33165,7 +33750,10 @@
       <c r="Y988" s="8"/>
       <c r="Z988" s="8"/>
     </row>
-    <row r="989" ht="15.75" customHeight="1" spans="2:26">
+    <row r="989" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A989" s="1" t="s">
+        <v>983</v>
+      </c>
       <c r="B989" s="8"/>
       <c r="C989" s="8"/>
       <c r="D989" s="8"/>
@@ -33192,7 +33780,10 @@
       <c r="Y989" s="8"/>
       <c r="Z989" s="8"/>
     </row>
-    <row r="990" ht="15.75" customHeight="1" spans="2:26">
+    <row r="990" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A990" s="1" t="s">
+        <v>984</v>
+      </c>
       <c r="B990" s="8"/>
       <c r="C990" s="8"/>
       <c r="D990" s="8"/>
@@ -33219,7 +33810,10 @@
       <c r="Y990" s="8"/>
       <c r="Z990" s="8"/>
     </row>
-    <row r="991" ht="15.75" customHeight="1" spans="2:26">
+    <row r="991" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A991" s="1" t="s">
+        <v>985</v>
+      </c>
       <c r="B991" s="8"/>
       <c r="C991" s="8"/>
       <c r="D991" s="8"/>
@@ -33246,7 +33840,10 @@
       <c r="Y991" s="8"/>
       <c r="Z991" s="8"/>
     </row>
-    <row r="992" ht="15.75" customHeight="1" spans="2:26">
+    <row r="992" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A992" s="1" t="s">
+        <v>986</v>
+      </c>
       <c r="B992" s="8"/>
       <c r="C992" s="8"/>
       <c r="D992" s="8"/>
@@ -33273,7 +33870,10 @@
       <c r="Y992" s="8"/>
       <c r="Z992" s="8"/>
     </row>
-    <row r="993" ht="15.75" customHeight="1" spans="2:26">
+    <row r="993" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A993" s="1" t="s">
+        <v>987</v>
+      </c>
       <c r="B993" s="8"/>
       <c r="C993" s="8"/>
       <c r="D993" s="8"/>
@@ -33300,7 +33900,10 @@
       <c r="Y993" s="8"/>
       <c r="Z993" s="8"/>
     </row>
-    <row r="994" ht="15.75" customHeight="1" spans="2:26">
+    <row r="994" ht="15.75" customHeight="1" spans="1:26">
+      <c r="A994" s="1" t="s">
+        <v>988</v>
+      </c>
       <c r="B994" s="8"/>
       <c r="C994" s="8"/>
       <c r="D994" s="8"/>
@@ -33327,32 +33930,145 @@
       <c r="Y994" s="8"/>
       <c r="Z994" s="8"/>
     </row>
-    <row r="995" ht="15.75" customHeight="1" spans="2:26">
-      <c r="B995" s="8"/>
-      <c r="C995" s="8"/>
-      <c r="D995" s="8"/>
-      <c r="E995" s="8"/>
-      <c r="F995" s="8"/>
-      <c r="G995" s="8"/>
-      <c r="H995" s="8"/>
-      <c r="I995" s="8"/>
-      <c r="J995" s="8"/>
-      <c r="K995" s="8"/>
-      <c r="L995" s="8"/>
-      <c r="M995" s="8"/>
-      <c r="N995" s="8"/>
-      <c r="O995" s="8"/>
-      <c r="P995" s="8"/>
-      <c r="Q995" s="8"/>
-      <c r="R995" s="8"/>
-      <c r="S995" s="8"/>
-      <c r="T995" s="8"/>
-      <c r="U995" s="8"/>
-      <c r="V995" s="8"/>
-      <c r="W995" s="8"/>
-      <c r="X995" s="8"/>
-      <c r="Y995" s="8"/>
-      <c r="Z995" s="8"/>
+    <row r="995" spans="1:1">
+      <c r="A995" s="1" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="996" spans="1:1">
+      <c r="A996" s="1" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="997" spans="1:1">
+      <c r="A997" s="1" t="s">
+        <v>991</v>
+      </c>
+    </row>
+    <row r="998" spans="1:1">
+      <c r="A998" s="1" t="s">
+        <v>992</v>
+      </c>
+    </row>
+    <row r="999" spans="1:1">
+      <c r="A999" s="1" t="s">
+        <v>993</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:1">
+      <c r="A1000" s="1" t="s">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:1">
+      <c r="A1001" s="1" t="s">
+        <v>995</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:1">
+      <c r="A1002" s="1" t="s">
+        <v>996</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:1">
+      <c r="A1003" s="1" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:1">
+      <c r="A1004" s="1" t="s">
+        <v>997</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:1">
+      <c r="A1005" s="1" t="s">
+        <v>998</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:1">
+      <c r="A1006" s="1" t="s">
+        <v>999</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:1">
+      <c r="A1007" s="1" t="s">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:1">
+      <c r="A1008" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:1">
+      <c r="A1009" s="1" t="s">
+        <v>1002</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:1">
+      <c r="A1010" s="1" t="s">
+        <v>1003</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:1">
+      <c r="A1011" s="1" t="s">
+        <v>1004</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:1">
+      <c r="A1012" s="1" t="s">
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:1">
+      <c r="A1013" s="1" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:1">
+      <c r="A1014" s="1" t="s">
+        <v>1006</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:1">
+      <c r="A1015" s="1" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:1">
+      <c r="A1016" s="1" t="s">
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:1">
+      <c r="A1017" s="1" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:1">
+      <c r="A1018" s="1" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:1">
+      <c r="A1019" s="1" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:1">
+      <c r="A1020" s="1" t="s">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:1">
+      <c r="A1021" s="1" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:1">
+      <c r="A1022" s="1" t="s">
+        <v>1014</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>